<commit_message>
DPE_GINI_P2 on "AGE_BASE" to identical/compatible
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_GINI_P2.xlsx
+++ b/rmonize/data_proc_elem/DPE_GINI_P2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C1775B-CA62-4757-87AD-C9C647139646}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2F30D0-EE43-4CB2-9555-28EE958EAC82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="329">
   <si>
     <t>Index</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>KIALTER_15</t>
-  </si>
-  <si>
-    <t>Franzi: KIALTER_15 is integer,  but we want decimal. So this can't be direct mapping, but needs recoding.</t>
   </si>
   <si>
     <t>EDU_LEVEL</t>
@@ -1600,9 +1597,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H102" sqref="H102"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1747,14 +1744,12 @@
       <c r="H4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="24" t="s">
-        <v>26</v>
-      </c>
+      <c r="I4" s="24"/>
       <c r="J4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="409.5">
@@ -1762,10 +1757,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
@@ -1774,22 +1769,22 @@
         <v>14</v>
       </c>
       <c r="F5" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="H5" s="18" t="s">
+        <v>322</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="18" t="s">
-        <v>323</v>
-      </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" ht="135">
@@ -1797,10 +1792,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -1809,22 +1804,22 @@
         <v>14</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>323</v>
+      </c>
+      <c r="I6" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>324</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>37</v>
-      </c>
       <c r="J6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="L6" s="2"/>
     </row>
@@ -1833,10 +1828,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>13</v>
@@ -1845,22 +1840,22 @@
         <v>14</v>
       </c>
       <c r="F7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" t="s">
         <v>40</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="I7" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="17" t="s">
-        <v>43</v>
-      </c>
       <c r="J7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" t="s">
         <v>32</v>
-      </c>
-      <c r="K7" t="s">
-        <v>33</v>
       </c>
       <c r="L7" s="7"/>
     </row>
@@ -1869,10 +1864,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>44</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>45</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -1881,16 +1876,16 @@
         <v>14</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="90">
@@ -1898,10 +1893,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>48</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>49</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>24</v>
@@ -1910,22 +1905,22 @@
         <v>14</v>
       </c>
       <c r="F9" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="23" t="s">
+        <v>318</v>
+      </c>
+      <c r="I9" s="15" t="s">
         <v>51</v>
-      </c>
-      <c r="H9" s="23" t="s">
-        <v>319</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>52</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1">
@@ -1933,10 +1928,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>13</v>
@@ -1945,19 +1940,19 @@
         <v>14</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K10" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1965,10 +1960,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
@@ -1977,16 +1972,16 @@
         <v>14</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1994,10 +1989,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -2006,16 +2001,16 @@
         <v>14</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -2023,10 +2018,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>13</v>
@@ -2035,16 +2030,16 @@
         <v>14</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="1" customFormat="1">
@@ -2052,10 +2047,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
@@ -2064,22 +2059,22 @@
         <v>14</v>
       </c>
       <c r="F14" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>16</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -2087,10 +2082,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
@@ -2098,19 +2093,19 @@
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K15" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -2118,26 +2113,26 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:13" s="1" customFormat="1">
@@ -2145,10 +2140,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
@@ -2158,16 +2153,16 @@
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:13" s="1" customFormat="1">
@@ -2175,10 +2170,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>13</v>
@@ -2187,16 +2182,16 @@
         <v>14</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -2204,26 +2199,26 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" t="s">
         <v>77</v>
-      </c>
-      <c r="C19" t="s">
-        <v>78</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -2231,10 +2226,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>24</v>
@@ -2243,7 +2238,7 @@
         <v>14</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>21</v>
@@ -2252,13 +2247,13 @@
         <v>21</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K20" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="K20" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -2266,10 +2261,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>24</v>
@@ -2278,7 +2273,7 @@
         <v>14</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>21</v>
@@ -2287,13 +2282,13 @@
         <v>21</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J21" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K21" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -2301,10 +2296,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>24</v>
@@ -2313,7 +2308,7 @@
         <v>14</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>21</v>
@@ -2322,13 +2317,13 @@
         <v>21</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K22" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="K22" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -2336,10 +2331,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>24</v>
@@ -2348,7 +2343,7 @@
         <v>14</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>21</v>
@@ -2357,13 +2352,13 @@
         <v>21</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J23" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K23" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -2371,26 +2366,26 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -2398,26 +2393,26 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>95</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -2425,26 +2420,26 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:13" s="1" customFormat="1">
@@ -2452,10 +2447,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>13</v>
@@ -2464,19 +2459,19 @@
         <v>14</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>16</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:13" s="1" customFormat="1">
@@ -2484,10 +2479,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>13</v>
@@ -2497,17 +2492,17 @@
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I28" s="10"/>
       <c r="J28" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M28" s="2"/>
     </row>
@@ -2516,10 +2511,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>13</v>
@@ -2528,22 +2523,22 @@
         <v>14</v>
       </c>
       <c r="F29" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G29" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H29" s="20" t="s">
+        <v>324</v>
+      </c>
+      <c r="I29" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="G29" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="H29" s="20" t="s">
-        <v>325</v>
-      </c>
-      <c r="I29" s="21" t="s">
-        <v>106</v>
-      </c>
       <c r="J29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K29" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="M29" s="7"/>
     </row>
@@ -2552,10 +2547,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>108</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
@@ -2563,16 +2558,16 @@
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -2580,26 +2575,26 @@
         <v>30</v>
       </c>
       <c r="B31" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>110</v>
       </c>
       <c r="D31" s="14"/>
       <c r="E31" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -2607,26 +2602,26 @@
         <v>31</v>
       </c>
       <c r="B32" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -2634,26 +2629,26 @@
         <v>32</v>
       </c>
       <c r="B33" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -2661,26 +2656,26 @@
         <v>33</v>
       </c>
       <c r="B34" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>116</v>
       </c>
       <c r="D34" s="14"/>
       <c r="E34" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -2688,26 +2683,26 @@
         <v>34</v>
       </c>
       <c r="B35" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>118</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -2715,26 +2710,26 @@
         <v>35</v>
       </c>
       <c r="B36" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>120</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -2742,26 +2737,26 @@
         <v>36</v>
       </c>
       <c r="B37" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -2769,26 +2764,26 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="D38" s="14"/>
       <c r="E38" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -2796,26 +2791,26 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
+        <v>124</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>126</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -2823,26 +2818,26 @@
         <v>39</v>
       </c>
       <c r="B40" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -2850,26 +2845,26 @@
         <v>40</v>
       </c>
       <c r="B41" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="D41" s="14"/>
       <c r="E41" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -2877,26 +2872,26 @@
         <v>41</v>
       </c>
       <c r="B42" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>131</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>132</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -2904,26 +2899,26 @@
         <v>42</v>
       </c>
       <c r="B43" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>134</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -2931,26 +2926,26 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>134</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>136</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -2958,26 +2953,26 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>136</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>138</v>
       </c>
       <c r="D45" s="14"/>
       <c r="E45" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -2985,26 +2980,26 @@
         <v>45</v>
       </c>
       <c r="B46" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>140</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -3012,25 +3007,25 @@
         <v>46</v>
       </c>
       <c r="B47" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>142</v>
-      </c>
       <c r="E47" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -3038,25 +3033,25 @@
         <v>47</v>
       </c>
       <c r="B48" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>144</v>
-      </c>
       <c r="E48" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -3064,25 +3059,25 @@
         <v>48</v>
       </c>
       <c r="B49" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C49" s="5" t="s">
-        <v>146</v>
-      </c>
       <c r="E49" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -3090,25 +3085,25 @@
         <v>49</v>
       </c>
       <c r="B50" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C50" s="5" t="s">
-        <v>148</v>
-      </c>
       <c r="E50" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -3116,25 +3111,25 @@
         <v>50</v>
       </c>
       <c r="B51" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>150</v>
-      </c>
       <c r="E51" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -3142,25 +3137,25 @@
         <v>51</v>
       </c>
       <c r="B52" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="E52" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -3168,25 +3163,25 @@
         <v>52</v>
       </c>
       <c r="B53" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>154</v>
-      </c>
       <c r="E53" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -3194,25 +3189,25 @@
         <v>53</v>
       </c>
       <c r="B54" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C54" s="4" t="s">
-        <v>156</v>
-      </c>
       <c r="E54" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -3220,25 +3215,25 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
+        <v>156</v>
+      </c>
+      <c r="C55" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>158</v>
-      </c>
       <c r="E55" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -3246,25 +3241,25 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
+        <v>158</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>160</v>
-      </c>
       <c r="E56" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -3272,25 +3267,25 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
+        <v>160</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C57" s="4" t="s">
-        <v>162</v>
-      </c>
       <c r="E57" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="58" spans="1:11" s="1" customFormat="1">
@@ -3298,26 +3293,26 @@
         <v>57</v>
       </c>
       <c r="B58" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C58" s="5" t="s">
         <v>163</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>164</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F58" s="15"/>
       <c r="G58" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:11" s="6" customFormat="1">
@@ -3325,25 +3320,25 @@
         <v>58</v>
       </c>
       <c r="B59" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C59" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="C59" s="4" t="s">
-        <v>166</v>
-      </c>
       <c r="E59" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" spans="1:11" s="1" customFormat="1">
@@ -3351,16 +3346,16 @@
         <v>59</v>
       </c>
       <c r="B60" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="E60" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F60" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>169</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>21</v>
@@ -3380,25 +3375,25 @@
         <v>60</v>
       </c>
       <c r="B61" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C61" s="4" t="s">
-        <v>171</v>
-      </c>
       <c r="E61" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -3406,25 +3401,25 @@
         <v>61</v>
       </c>
       <c r="B62" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="C62" s="4" t="s">
-        <v>173</v>
-      </c>
       <c r="E62" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="63" spans="1:11">
@@ -3432,25 +3427,25 @@
         <v>62</v>
       </c>
       <c r="B63" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C63" s="4" t="s">
-        <v>175</v>
-      </c>
       <c r="E63" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -3458,25 +3453,25 @@
         <v>63</v>
       </c>
       <c r="B64" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C64" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C64" s="4" t="s">
-        <v>177</v>
-      </c>
       <c r="E64" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="65" spans="1:11">
@@ -3484,16 +3479,16 @@
         <v>64</v>
       </c>
       <c r="B65" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C65" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="E65" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F65" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F65" s="8" t="s">
-        <v>180</v>
       </c>
       <c r="G65" s="8" t="s">
         <v>21</v>
@@ -3511,10 +3506,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C66" s="14" t="s">
         <v>181</v>
-      </c>
-      <c r="C66" s="14" t="s">
-        <v>182</v>
       </c>
       <c r="D66" s="8" t="s">
         <v>24</v>
@@ -3523,7 +3518,7 @@
         <v>14</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G66" s="8" t="s">
         <v>21</v>
@@ -3542,10 +3537,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="D67" s="8" t="s">
         <v>24</v>
@@ -3554,7 +3549,7 @@
         <v>14</v>
       </c>
       <c r="F67" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G67" s="8" t="s">
         <v>21</v>
@@ -3573,17 +3568,17 @@
         <v>67</v>
       </c>
       <c r="B68" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="D68" s="8"/>
       <c r="E68" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G68" s="8" t="s">
         <v>21</v>
@@ -3594,7 +3589,7 @@
         <v>16</v>
       </c>
       <c r="K68" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="69" spans="1:11" s="6" customFormat="1">
@@ -3602,10 +3597,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="D69" s="8"/>
       <c r="E69" s="8" t="s">
@@ -3613,17 +3608,17 @@
       </c>
       <c r="F69" s="11"/>
       <c r="G69" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I69"/>
       <c r="J69" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -3631,10 +3626,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C70" s="14" t="s">
         <v>192</v>
-      </c>
-      <c r="C70" s="14" t="s">
-        <v>193</v>
       </c>
       <c r="D70" s="8"/>
       <c r="E70" s="8" t="s">
@@ -3642,15 +3637,15 @@
       </c>
       <c r="F70" s="8"/>
       <c r="G70" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H70" s="8"/>
       <c r="I70" s="8"/>
       <c r="J70" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K70" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -3658,10 +3653,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C71" s="14" t="s">
         <v>194</v>
-      </c>
-      <c r="C71" s="14" t="s">
-        <v>195</v>
       </c>
       <c r="D71" s="8"/>
       <c r="E71" s="8" t="s">
@@ -3669,15 +3664,15 @@
       </c>
       <c r="F71" s="8"/>
       <c r="G71" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H71" s="8"/>
       <c r="I71" s="8"/>
       <c r="J71" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K71" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="72" spans="1:11">
@@ -3685,10 +3680,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C72" s="14" t="s">
         <v>196</v>
-      </c>
-      <c r="C72" s="14" t="s">
-        <v>197</v>
       </c>
       <c r="D72" s="8"/>
       <c r="E72" s="8" t="s">
@@ -3696,15 +3691,15 @@
       </c>
       <c r="F72" s="8"/>
       <c r="G72" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H72" s="8"/>
       <c r="I72" s="8"/>
       <c r="J72" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K72" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="73" spans="1:11">
@@ -3712,10 +3707,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C73" s="14" t="s">
         <v>198</v>
-      </c>
-      <c r="C73" s="14" t="s">
-        <v>199</v>
       </c>
       <c r="D73" s="8"/>
       <c r="E73" s="8" t="s">
@@ -3723,15 +3718,15 @@
       </c>
       <c r="F73" s="8"/>
       <c r="G73" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H73" s="8"/>
       <c r="I73" s="8"/>
       <c r="J73" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K73" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="1:11">
@@ -3739,10 +3734,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="C74" s="14" t="s">
         <v>200</v>
-      </c>
-      <c r="C74" s="14" t="s">
-        <v>201</v>
       </c>
       <c r="D74" s="8" t="s">
         <v>24</v>
@@ -3752,15 +3747,15 @@
       </c>
       <c r="F74" s="8"/>
       <c r="G74" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H74" s="8"/>
       <c r="I74" s="8"/>
       <c r="J74" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K74" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="75" spans="1:11">
@@ -3768,10 +3763,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="C75" s="14" t="s">
         <v>202</v>
-      </c>
-      <c r="C75" s="14" t="s">
-        <v>203</v>
       </c>
       <c r="D75" s="8" t="s">
         <v>24</v>
@@ -3780,7 +3775,7 @@
         <v>14</v>
       </c>
       <c r="F75" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G75" s="8" t="s">
         <v>21</v>
@@ -3799,10 +3794,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="D76" s="8" t="s">
         <v>24</v>
@@ -3812,15 +3807,15 @@
       </c>
       <c r="F76" s="8"/>
       <c r="G76" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H76" s="8"/>
       <c r="I76" s="8"/>
       <c r="J76" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K76" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="77" spans="1:11" s="1" customFormat="1">
@@ -3828,10 +3823,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>208</v>
       </c>
       <c r="D77" s="8" t="s">
         <v>24</v>
@@ -3840,20 +3835,20 @@
         <v>14</v>
       </c>
       <c r="F77" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G77" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H77" s="8"/>
       <c r="I77" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J77" s="8" t="s">
         <v>16</v>
       </c>
       <c r="K77" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="78" spans="1:11" s="1" customFormat="1">
@@ -3861,10 +3856,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="D78" s="8" t="s">
         <v>24</v>
@@ -3873,7 +3868,7 @@
         <v>14</v>
       </c>
       <c r="F78" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G78" s="8" t="s">
         <v>21</v>
@@ -3892,10 +3887,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C79" s="14" t="s">
         <v>213</v>
-      </c>
-      <c r="C79" s="14" t="s">
-        <v>214</v>
       </c>
       <c r="D79" s="8" t="s">
         <v>24</v>
@@ -3904,7 +3899,7 @@
         <v>14</v>
       </c>
       <c r="F79" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G79" s="8" t="s">
         <v>21</v>
@@ -3923,10 +3918,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C80" s="14" t="s">
         <v>216</v>
-      </c>
-      <c r="C80" s="14" t="s">
-        <v>217</v>
       </c>
       <c r="D80" s="8" t="s">
         <v>24</v>
@@ -3935,13 +3930,13 @@
         <v>14</v>
       </c>
       <c r="F80" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="G80" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H80" s="8" t="s">
         <v>218</v>
-      </c>
-      <c r="G80" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H80" s="8" t="s">
-        <v>219</v>
       </c>
       <c r="I80" s="8"/>
       <c r="J80" s="8" t="s">
@@ -3956,10 +3951,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C81" s="14" t="s">
         <v>220</v>
-      </c>
-      <c r="C81" s="14" t="s">
-        <v>221</v>
       </c>
       <c r="D81" s="8" t="s">
         <v>24</v>
@@ -3968,13 +3963,13 @@
         <v>14</v>
       </c>
       <c r="F81" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="G81" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H81" s="8" t="s">
         <v>222</v>
-      </c>
-      <c r="G81" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H81" s="8" t="s">
-        <v>223</v>
       </c>
       <c r="I81" s="8"/>
       <c r="J81" s="8" t="s">
@@ -3989,10 +3984,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="C82" s="14" t="s">
         <v>224</v>
-      </c>
-      <c r="C82" s="14" t="s">
-        <v>225</v>
       </c>
       <c r="D82" s="8" t="s">
         <v>24</v>
@@ -4001,13 +3996,13 @@
         <v>14</v>
       </c>
       <c r="F82" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="G82" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H82" s="8" t="s">
         <v>226</v>
-      </c>
-      <c r="G82" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H82" s="8" t="s">
-        <v>227</v>
       </c>
       <c r="I82" s="8"/>
       <c r="J82" s="8" t="s">
@@ -4022,10 +4017,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C83" s="14" t="s">
         <v>228</v>
-      </c>
-      <c r="C83" s="14" t="s">
-        <v>229</v>
       </c>
       <c r="D83" s="8" t="s">
         <v>24</v>
@@ -4034,13 +4029,13 @@
         <v>14</v>
       </c>
       <c r="F83" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="G83" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H83" s="8" t="s">
         <v>230</v>
-      </c>
-      <c r="G83" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H83" s="8" t="s">
-        <v>231</v>
       </c>
       <c r="I83" s="8"/>
       <c r="J83" s="8" t="s">
@@ -4055,10 +4050,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="C84" s="14" t="s">
         <v>232</v>
-      </c>
-      <c r="C84" s="14" t="s">
-        <v>233</v>
       </c>
       <c r="D84" s="8" t="s">
         <v>24</v>
@@ -4067,13 +4062,13 @@
         <v>14</v>
       </c>
       <c r="F84" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="G84" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H84" s="8" t="s">
         <v>234</v>
-      </c>
-      <c r="G84" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H84" s="8" t="s">
-        <v>235</v>
       </c>
       <c r="I84" s="8"/>
       <c r="J84" s="8" t="s">
@@ -4088,10 +4083,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="C85" s="14" t="s">
         <v>236</v>
-      </c>
-      <c r="C85" s="14" t="s">
-        <v>237</v>
       </c>
       <c r="D85" s="8" t="s">
         <v>24</v>
@@ -4100,13 +4095,13 @@
         <v>14</v>
       </c>
       <c r="F85" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="G85" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H85" s="8" t="s">
         <v>238</v>
-      </c>
-      <c r="G85" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H85" s="8" t="s">
-        <v>239</v>
       </c>
       <c r="I85" s="8"/>
       <c r="J85" s="8" t="s">
@@ -4121,10 +4116,10 @@
         <v>85</v>
       </c>
       <c r="B86" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C86" s="14" t="s">
         <v>240</v>
-      </c>
-      <c r="C86" s="14" t="s">
-        <v>241</v>
       </c>
       <c r="D86" s="8" t="s">
         <v>24</v>
@@ -4133,13 +4128,13 @@
         <v>14</v>
       </c>
       <c r="F86" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="G86" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H86" s="8" t="s">
         <v>242</v>
-      </c>
-      <c r="G86" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H86" s="8" t="s">
-        <v>243</v>
       </c>
       <c r="I86" s="8"/>
       <c r="J86" s="8" t="s">
@@ -4154,10 +4149,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="C87" s="14" t="s">
         <v>244</v>
-      </c>
-      <c r="C87" s="14" t="s">
-        <v>245</v>
       </c>
       <c r="D87" s="8" t="s">
         <v>24</v>
@@ -4166,13 +4161,13 @@
         <v>14</v>
       </c>
       <c r="F87" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="G87" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H87" s="8" t="s">
         <v>246</v>
-      </c>
-      <c r="G87" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H87" s="8" t="s">
-        <v>247</v>
       </c>
       <c r="I87" s="8"/>
       <c r="J87" s="8" t="s">
@@ -4187,10 +4182,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="C88" s="14" t="s">
         <v>248</v>
-      </c>
-      <c r="C88" s="14" t="s">
-        <v>249</v>
       </c>
       <c r="D88" s="8" t="s">
         <v>24</v>
@@ -4200,15 +4195,15 @@
       </c>
       <c r="F88" s="8"/>
       <c r="G88" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H88" s="8"/>
       <c r="I88" s="8"/>
       <c r="J88" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K88" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="89" spans="1:11">
@@ -4216,10 +4211,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="C89" s="14" t="s">
         <v>250</v>
-      </c>
-      <c r="C89" s="14" t="s">
-        <v>251</v>
       </c>
       <c r="D89" s="8" t="s">
         <v>24</v>
@@ -4229,15 +4224,15 @@
       </c>
       <c r="F89" s="8"/>
       <c r="G89" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H89" s="8"/>
       <c r="I89" s="8"/>
       <c r="J89" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K89" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="90" spans="1:11">
@@ -4245,10 +4240,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="C90" s="14" t="s">
         <v>252</v>
-      </c>
-      <c r="C90" s="14" t="s">
-        <v>253</v>
       </c>
       <c r="D90" s="8" t="s">
         <v>24</v>
@@ -4258,15 +4253,15 @@
       </c>
       <c r="F90" s="8"/>
       <c r="G90" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H90" s="8"/>
       <c r="I90" s="8"/>
       <c r="J90" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K90" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="91" spans="1:11">
@@ -4274,10 +4269,10 @@
         <v>90</v>
       </c>
       <c r="B91" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="C91" s="14" t="s">
         <v>254</v>
-      </c>
-      <c r="C91" s="14" t="s">
-        <v>255</v>
       </c>
       <c r="D91" s="8" t="s">
         <v>24</v>
@@ -4286,13 +4281,13 @@
         <v>14</v>
       </c>
       <c r="F91" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="G91" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H91" s="8" t="s">
         <v>256</v>
-      </c>
-      <c r="G91" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H91" s="8" t="s">
-        <v>257</v>
       </c>
       <c r="I91" s="8"/>
       <c r="J91" s="8" t="s">
@@ -4307,10 +4302,10 @@
         <v>91</v>
       </c>
       <c r="B92" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C92" s="14" t="s">
         <v>258</v>
-      </c>
-      <c r="C92" s="14" t="s">
-        <v>259</v>
       </c>
       <c r="D92" s="8" t="s">
         <v>24</v>
@@ -4319,13 +4314,13 @@
         <v>14</v>
       </c>
       <c r="F92" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="G92" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H92" s="8" t="s">
         <v>260</v>
-      </c>
-      <c r="G92" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H92" s="8" t="s">
-        <v>261</v>
       </c>
       <c r="I92" s="8"/>
       <c r="J92" s="8" t="s">
@@ -4340,10 +4335,10 @@
         <v>92</v>
       </c>
       <c r="B93" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>263</v>
       </c>
       <c r="D93" s="8" t="s">
         <v>24</v>
@@ -4352,13 +4347,13 @@
         <v>14</v>
       </c>
       <c r="F93" s="15" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I93" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J93" s="8" t="s">
         <v>16</v>
@@ -4372,10 +4367,10 @@
         <v>93</v>
       </c>
       <c r="B94" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>267</v>
       </c>
       <c r="D94" s="8" t="s">
         <v>24</v>
@@ -4384,13 +4379,13 @@
         <v>14</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I94" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J94" s="8" t="s">
         <v>16</v>
@@ -4404,10 +4399,10 @@
         <v>94</v>
       </c>
       <c r="B95" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="C95" s="14" t="s">
         <v>269</v>
-      </c>
-      <c r="C95" s="14" t="s">
-        <v>270</v>
       </c>
       <c r="D95" s="8" t="s">
         <v>24</v>
@@ -4416,13 +4411,13 @@
         <v>14</v>
       </c>
       <c r="F95" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="G95" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H95" s="8" t="s">
         <v>271</v>
-      </c>
-      <c r="G95" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H95" s="8" t="s">
-        <v>272</v>
       </c>
       <c r="I95" s="8"/>
       <c r="J95" s="8" t="s">
@@ -4437,10 +4432,10 @@
         <v>95</v>
       </c>
       <c r="B96" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C96" s="14" t="s">
         <v>273</v>
-      </c>
-      <c r="C96" s="14" t="s">
-        <v>274</v>
       </c>
       <c r="D96" s="8" t="s">
         <v>24</v>
@@ -4449,13 +4444,13 @@
         <v>14</v>
       </c>
       <c r="F96" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="G96" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H96" s="8" t="s">
         <v>275</v>
-      </c>
-      <c r="G96" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H96" s="8" t="s">
-        <v>276</v>
       </c>
       <c r="I96" s="8"/>
       <c r="J96" s="8" t="s">
@@ -4470,10 +4465,10 @@
         <v>96</v>
       </c>
       <c r="B97" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="C97" s="16" t="s">
         <v>277</v>
-      </c>
-      <c r="C97" s="16" t="s">
-        <v>278</v>
       </c>
       <c r="D97" s="8" t="s">
         <v>24</v>
@@ -4482,20 +4477,20 @@
         <v>14</v>
       </c>
       <c r="F97" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="G97" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H97" s="8" t="s">
         <v>279</v>
-      </c>
-      <c r="G97" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H97" s="8" t="s">
-        <v>280</v>
       </c>
       <c r="I97" s="8"/>
       <c r="J97" s="8" t="s">
         <v>16</v>
       </c>
       <c r="K97" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="98" spans="1:11">
@@ -4503,10 +4498,10 @@
         <v>97</v>
       </c>
       <c r="B98" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="C98" s="13" t="s">
         <v>281</v>
-      </c>
-      <c r="C98" s="13" t="s">
-        <v>282</v>
       </c>
       <c r="D98" s="8" t="s">
         <v>24</v>
@@ -4515,20 +4510,20 @@
         <v>14</v>
       </c>
       <c r="F98" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="G98" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H98" s="8" t="s">
         <v>283</v>
-      </c>
-      <c r="G98" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H98" s="8" t="s">
-        <v>284</v>
       </c>
       <c r="I98" s="8"/>
       <c r="J98" s="8" t="s">
         <v>16</v>
       </c>
       <c r="K98" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="99" spans="1:11">
@@ -4536,10 +4531,10 @@
         <v>98</v>
       </c>
       <c r="B99" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C99" s="13" t="s">
         <v>285</v>
-      </c>
-      <c r="C99" s="13" t="s">
-        <v>286</v>
       </c>
       <c r="D99" s="8" t="s">
         <v>24</v>
@@ -4548,20 +4543,20 @@
         <v>14</v>
       </c>
       <c r="F99" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="G99" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H99" s="8" t="s">
         <v>287</v>
-      </c>
-      <c r="G99" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H99" s="8" t="s">
-        <v>288</v>
       </c>
       <c r="I99" s="8"/>
       <c r="J99" s="8" t="s">
         <v>16</v>
       </c>
       <c r="K99" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="100" spans="1:11">
@@ -4569,10 +4564,10 @@
         <v>99</v>
       </c>
       <c r="B100" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C100" s="13" t="s">
         <v>289</v>
-      </c>
-      <c r="C100" s="13" t="s">
-        <v>290</v>
       </c>
       <c r="D100" s="8" t="s">
         <v>24</v>
@@ -4581,20 +4576,20 @@
         <v>14</v>
       </c>
       <c r="F100" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="G100" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H100" s="8" t="s">
         <v>291</v>
-      </c>
-      <c r="G100" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H100" s="8" t="s">
-        <v>292</v>
       </c>
       <c r="I100" s="8"/>
       <c r="J100" s="8" t="s">
         <v>16</v>
       </c>
       <c r="K100" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="101" spans="1:11">
@@ -4602,10 +4597,10 @@
         <v>100</v>
       </c>
       <c r="B101" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C101" s="13" t="s">
         <v>293</v>
-      </c>
-      <c r="C101" s="13" t="s">
-        <v>294</v>
       </c>
       <c r="D101" s="8" t="s">
         <v>24</v>
@@ -4615,15 +4610,15 @@
       </c>
       <c r="F101" s="8"/>
       <c r="G101" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H101" s="8"/>
       <c r="I101" s="8"/>
       <c r="J101" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K101" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="102" spans="1:11">
@@ -4631,10 +4626,10 @@
         <v>101</v>
       </c>
       <c r="B102" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C102" s="13" t="s">
         <v>295</v>
-      </c>
-      <c r="C102" s="13" t="s">
-        <v>296</v>
       </c>
       <c r="D102" s="8" t="s">
         <v>24</v>
@@ -4643,20 +4638,20 @@
         <v>14</v>
       </c>
       <c r="F102" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="G102" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H102" s="8" t="s">
         <v>297</v>
-      </c>
-      <c r="G102" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H102" s="8" t="s">
-        <v>298</v>
       </c>
       <c r="I102" s="8"/>
       <c r="J102" s="8" t="s">
         <v>16</v>
       </c>
       <c r="K102" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="103" spans="1:11">
@@ -4664,10 +4659,10 @@
         <v>102</v>
       </c>
       <c r="B103" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="C103" s="14" t="s">
         <v>299</v>
-      </c>
-      <c r="C103" s="14" t="s">
-        <v>300</v>
       </c>
       <c r="D103" s="8" t="s">
         <v>24</v>
@@ -4677,15 +4672,15 @@
       </c>
       <c r="F103" s="8"/>
       <c r="G103" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H103" s="8"/>
       <c r="I103" s="8"/>
       <c r="J103" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K103" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="104" spans="1:11" ht="60">
@@ -4693,10 +4688,10 @@
         <v>103</v>
       </c>
       <c r="B104" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="C104" s="16" t="s">
         <v>301</v>
-      </c>
-      <c r="C104" s="16" t="s">
-        <v>302</v>
       </c>
       <c r="D104" s="8" t="s">
         <v>24</v>
@@ -4705,20 +4700,20 @@
         <v>14</v>
       </c>
       <c r="F104" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="G104" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H104" s="18" t="s">
         <v>326</v>
-      </c>
-      <c r="G104" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H104" s="18" t="s">
-        <v>327</v>
       </c>
       <c r="I104" s="8"/>
       <c r="J104" s="8" t="s">
         <v>16</v>
       </c>
       <c r="K104" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="105" spans="1:11">
@@ -4726,10 +4721,10 @@
         <v>104</v>
       </c>
       <c r="B105" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="C105" s="13" t="s">
         <v>303</v>
-      </c>
-      <c r="C105" s="13" t="s">
-        <v>304</v>
       </c>
       <c r="D105" s="8" t="s">
         <v>24</v>
@@ -4738,13 +4733,13 @@
         <v>14</v>
       </c>
       <c r="F105" s="18" t="s">
+        <v>327</v>
+      </c>
+      <c r="G105" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H105" s="8" t="s">
         <v>328</v>
-      </c>
-      <c r="G105" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H105" s="8" t="s">
-        <v>329</v>
       </c>
       <c r="I105" s="8"/>
       <c r="J105" s="8" t="s">
@@ -4759,10 +4754,10 @@
         <v>105</v>
       </c>
       <c r="B106" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="C106" s="13" t="s">
         <v>305</v>
-      </c>
-      <c r="C106" s="13" t="s">
-        <v>306</v>
       </c>
       <c r="D106" s="8" t="s">
         <v>24</v>
@@ -4771,20 +4766,20 @@
         <v>14</v>
       </c>
       <c r="F106" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="G106" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H106" s="8" t="s">
         <v>307</v>
-      </c>
-      <c r="G106" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H106" s="8" t="s">
-        <v>308</v>
       </c>
       <c r="I106" s="8"/>
       <c r="J106" s="8" t="s">
         <v>16</v>
       </c>
       <c r="K106" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="107" spans="1:11">
@@ -4792,10 +4787,10 @@
         <v>106</v>
       </c>
       <c r="B107" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="C107" s="13" t="s">
         <v>309</v>
-      </c>
-      <c r="C107" s="13" t="s">
-        <v>310</v>
       </c>
       <c r="D107" s="8" t="s">
         <v>24</v>
@@ -4805,15 +4800,15 @@
       </c>
       <c r="F107" s="8"/>
       <c r="G107" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H107" s="8"/>
       <c r="I107" s="8"/>
       <c r="J107" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K107" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="108" spans="1:11">
@@ -4821,10 +4816,10 @@
         <v>107</v>
       </c>
       <c r="B108" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="C108" s="13" t="s">
         <v>311</v>
-      </c>
-      <c r="C108" s="13" t="s">
-        <v>312</v>
       </c>
       <c r="D108" s="8" t="s">
         <v>24</v>
@@ -4833,7 +4828,7 @@
         <v>14</v>
       </c>
       <c r="F108" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G108" s="8" t="s">
         <v>21</v>
@@ -4852,10 +4847,10 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
+        <v>313</v>
+      </c>
+      <c r="C109" t="s">
         <v>314</v>
-      </c>
-      <c r="C109" t="s">
-        <v>315</v>
       </c>
       <c r="D109" s="27" t="s">
         <v>13</v>
@@ -4864,16 +4859,16 @@
         <v>14</v>
       </c>
       <c r="F109" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="G109" s="3" t="s">
         <v>316</v>
-      </c>
-      <c r="G109" s="3" t="s">
-        <v>317</v>
       </c>
       <c r="H109">
         <v>1</v>
       </c>
       <c r="I109" s="27" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J109" s="14" t="s">
         <v>16</v>
@@ -4955,6 +4950,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -5195,15 +5199,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -5217,6 +5212,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{398CA3EE-638E-435F-8CA6-D67A7B863103}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2AE2FD3-517E-4530-8BC5-1FF35C67F615}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5235,14 +5238,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{398CA3EE-638E-435F-8CA6-D67A7B863103}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF2265-5030-4B54-A34F-4798AFD4DA4C}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
updated Dataschema P2 to include "[years]" in all AGE related variables and DPEs accordingly
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_GINI_P2.xlsx
+++ b/rmonize/data_proc_elem/DPE_GINI_P2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5EAE45-A677-4DD9-8344-AE433300C554}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52413BDC-9100-4D8F-9686-E4AF9739279C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22050" windowHeight="8100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -379,9 +379,6 @@
     <t>AGE_CVD</t>
   </si>
   <si>
-    <t>Age at diagnosis of CVD</t>
-  </si>
-  <si>
     <t>INC_ANGINA</t>
   </si>
   <si>
@@ -391,9 +388,6 @@
     <t>AGE_ANGINA</t>
   </si>
   <si>
-    <t>Age at diagnosis of angina pectoris</t>
-  </si>
-  <si>
     <t>INC_MI</t>
   </si>
   <si>
@@ -403,9 +397,6 @@
     <t>AGE_MI</t>
   </si>
   <si>
-    <t>Age at diagnosis of myocardial infarction</t>
-  </si>
-  <si>
     <t>INC_STR</t>
   </si>
   <si>
@@ -415,9 +406,6 @@
     <t>AGE_STR</t>
   </si>
   <si>
-    <t>Age at diagnosis of stroke</t>
-  </si>
-  <si>
     <t>INC_ISC_STR</t>
   </si>
   <si>
@@ -427,9 +415,6 @@
     <t>AGE_ISC_STR</t>
   </si>
   <si>
-    <t>Age at diagnosis of cerebral infarction (ischaemic stroke)</t>
-  </si>
-  <si>
     <t>INC_HAEMO_STR</t>
   </si>
   <si>
@@ -439,9 +424,6 @@
     <t>AGE_HAEMO_STR</t>
   </si>
   <si>
-    <t>Age at diagnosis of haemorrhagic stroke</t>
-  </si>
-  <si>
     <t>INC_HYP</t>
   </si>
   <si>
@@ -451,9 +433,6 @@
     <t>AGE_HYP</t>
   </si>
   <si>
-    <t>Age at diagnosis of essential hypertension</t>
-  </si>
-  <si>
     <t>INC_HF</t>
   </si>
   <si>
@@ -463,9 +442,6 @@
     <t>AGE_HF</t>
   </si>
   <si>
-    <t>Age at diagnosis of heart failure</t>
-  </si>
-  <si>
     <t>INC_DIAB2</t>
   </si>
   <si>
@@ -475,9 +451,6 @@
     <t>AGE_DIAB2</t>
   </si>
   <si>
-    <t>Age at diagnosis of diabetes mellitus type 2</t>
-  </si>
-  <si>
     <t>INC_CANCER</t>
   </si>
   <si>
@@ -490,9 +463,6 @@
     <t>AGE_CANCER</t>
   </si>
   <si>
-    <t>Age at diagnosis of cancer</t>
-  </si>
-  <si>
     <t>maligjeadalt_15</t>
   </si>
   <si>
@@ -503,9 +473,6 @@
   </si>
   <si>
     <t>AGE_DEATH</t>
-  </si>
-  <si>
-    <t>Age at time of death</t>
   </si>
   <si>
     <t>VITAL_ST_CVD</t>
@@ -1105,6 +1072,39 @@
   </si>
   <si>
     <t>FFQGL_15</t>
+  </si>
+  <si>
+    <t>Age at diagnosis of CVD [years]</t>
+  </si>
+  <si>
+    <t>Age at diagnosis of angina pectoris [years]</t>
+  </si>
+  <si>
+    <t>Age at diagnosis of myocardial infarction [years]</t>
+  </si>
+  <si>
+    <t>Age at diagnosis of stroke [years]</t>
+  </si>
+  <si>
+    <t>Age at diagnosis of cerebral infarction (ischaemic stroke) [years]</t>
+  </si>
+  <si>
+    <t>Age at diagnosis of haemorrhagic stroke [years]</t>
+  </si>
+  <si>
+    <t>Age at diagnosis of essential hypertension [years]</t>
+  </si>
+  <si>
+    <t>Age at diagnosis of heart failure [years]</t>
+  </si>
+  <si>
+    <t>Age at diagnosis of diabetes mellitus type 2 [years]</t>
+  </si>
+  <si>
+    <t>Age at diagnosis of cancer [years]</t>
+  </si>
+  <si>
+    <t>Age at time of death [years]</t>
   </si>
 </sst>
 </file>
@@ -1588,9 +1588,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F90" sqref="F90"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,7 +1608,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -1715,7 +1715,7 @@
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="D4" t="s">
         <v>22</v>
@@ -1763,7 +1763,7 @@
         <v>27</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>28</v>
@@ -1798,7 +1798,7 @@
         <v>27</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="I6" s="16" t="s">
         <v>34</v>
@@ -1855,7 +1855,7 @@
         <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
@@ -1884,7 +1884,7 @@
         <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
@@ -1899,7 +1899,7 @@
         <v>46</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="I9" s="13"/>
       <c r="J9" s="1" t="s">
@@ -1932,7 +1932,7 @@
         <v>38</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>29</v>
@@ -1949,7 +1949,7 @@
         <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
@@ -1978,7 +1978,7 @@
         <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="D12" t="s">
         <v>22</v>
@@ -2007,7 +2007,7 @@
         <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="D13" t="s">
         <v>22</v>
@@ -2051,7 +2051,7 @@
         <v>38</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>57</v>
@@ -2133,7 +2133,7 @@
         <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
@@ -2163,7 +2163,7 @@
         <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
@@ -2192,7 +2192,7 @@
         <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="D19" t="s">
         <v>22</v>
@@ -2221,7 +2221,7 @@
         <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -2256,7 +2256,7 @@
         <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="D21" t="s">
         <v>22</v>
@@ -2291,7 +2291,7 @@
         <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="D22" t="s">
         <v>22</v>
@@ -2326,7 +2326,7 @@
         <v>74</v>
       </c>
       <c r="C23" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="D23" t="s">
         <v>22</v>
@@ -2463,7 +2463,7 @@
         <v>38</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>15</v>
@@ -2527,7 +2527,7 @@
         <v>27</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="I29" s="18" t="s">
         <v>90</v>
@@ -2694,7 +2694,7 @@
         <v>101</v>
       </c>
       <c r="C35" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="D35" t="s">
         <v>12</v>
@@ -2723,7 +2723,7 @@
         <v>102</v>
       </c>
       <c r="C36" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="D36" t="s">
         <v>12</v>
@@ -2752,7 +2752,7 @@
         <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="D37" t="s">
         <v>12</v>
@@ -2868,7 +2868,7 @@
         <v>110</v>
       </c>
       <c r="C41" t="s">
-        <v>111</v>
+        <v>318</v>
       </c>
       <c r="D41" t="s">
         <v>22</v>
@@ -2894,10 +2894,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42" t="s">
         <v>112</v>
-      </c>
-      <c r="C42" t="s">
-        <v>113</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
@@ -2923,10 +2923,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C43" t="s">
-        <v>115</v>
+        <v>319</v>
       </c>
       <c r="D43" t="s">
         <v>22</v>
@@ -2952,10 +2952,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C44" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
@@ -2981,10 +2981,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C45" t="s">
-        <v>119</v>
+        <v>320</v>
       </c>
       <c r="D45" t="s">
         <v>22</v>
@@ -3010,10 +3010,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C46" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D46" t="s">
         <v>12</v>
@@ -3039,10 +3039,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C47" t="s">
-        <v>123</v>
+        <v>321</v>
       </c>
       <c r="D47" t="s">
         <v>22</v>
@@ -3068,10 +3068,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C48" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D48" t="s">
         <v>12</v>
@@ -3097,10 +3097,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C49" t="s">
-        <v>127</v>
+        <v>322</v>
       </c>
       <c r="D49" t="s">
         <v>22</v>
@@ -3126,10 +3126,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C50" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D50" t="s">
         <v>12</v>
@@ -3155,10 +3155,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C51" t="s">
-        <v>131</v>
+        <v>323</v>
       </c>
       <c r="D51" t="s">
         <v>22</v>
@@ -3184,10 +3184,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C52" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
@@ -3213,10 +3213,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C53" t="s">
-        <v>135</v>
+        <v>324</v>
       </c>
       <c r="D53" t="s">
         <v>22</v>
@@ -3242,10 +3242,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C54" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D54" t="s">
         <v>12</v>
@@ -3271,10 +3271,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C55" t="s">
-        <v>139</v>
+        <v>325</v>
       </c>
       <c r="D55" t="s">
         <v>22</v>
@@ -3300,10 +3300,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C56" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D56" t="s">
         <v>12</v>
@@ -3329,10 +3329,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C57" t="s">
-        <v>143</v>
+        <v>326</v>
       </c>
       <c r="D57" t="s">
         <v>22</v>
@@ -3358,10 +3358,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C58" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D58" t="s">
         <v>12</v>
@@ -3388,13 +3388,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C59" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="D59" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>13</v>
@@ -3417,10 +3417,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C60" t="s">
-        <v>148</v>
+        <v>327</v>
       </c>
       <c r="D60" t="s">
         <v>22</v>
@@ -3429,7 +3429,7 @@
         <v>13</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>20</v>
@@ -3449,10 +3449,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C61" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="D61" t="s">
         <v>12</v>
@@ -3478,10 +3478,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C62" t="s">
-        <v>153</v>
+        <v>328</v>
       </c>
       <c r="D62" t="s">
         <v>22</v>
@@ -3507,10 +3507,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="C63" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="D63" t="s">
         <v>12</v>
@@ -3536,10 +3536,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="C64" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="D64" t="s">
         <v>12</v>
@@ -3565,10 +3565,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="C65" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="D65" t="s">
         <v>22</v>
@@ -3577,7 +3577,7 @@
         <v>13</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="G65" s="7" t="s">
         <v>20</v>
@@ -3597,10 +3597,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C66" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="D66" t="s">
         <v>22</v>
@@ -3609,7 +3609,7 @@
         <v>13</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="G66" s="7" t="s">
         <v>20</v>
@@ -3630,10 +3630,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="C67" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="D67" t="s">
         <v>22</v>
@@ -3642,7 +3642,7 @@
         <v>13</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="G67" s="7" t="s">
         <v>20</v>
@@ -3663,10 +3663,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="C68" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="D68" t="s">
         <v>22</v>
@@ -3675,7 +3675,7 @@
         <v>13</v>
       </c>
       <c r="F68" s="15" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="G68" s="7" t="s">
         <v>20</v>
@@ -3696,10 +3696,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C69" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="D69" t="s">
         <v>22</v>
@@ -3727,10 +3727,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C70" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="D70" t="s">
         <v>22</v>
@@ -3758,10 +3758,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C71" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="D71" t="s">
         <v>22</v>
@@ -3789,10 +3789,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C72" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="D72" t="s">
         <v>22</v>
@@ -3820,10 +3820,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="C73" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="D73" t="s">
         <v>22</v>
@@ -3851,10 +3851,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C74" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="D74" t="s">
         <v>22</v>
@@ -3882,10 +3882,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C75" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="D75" t="s">
         <v>22</v>
@@ -3894,7 +3894,7 @@
         <v>13</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="G75" s="7" t="s">
         <v>20</v>
@@ -3915,10 +3915,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C76" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="D76" t="s">
         <v>22</v>
@@ -3946,10 +3946,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="C77" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="D77" t="s">
         <v>22</v>
@@ -3958,7 +3958,7 @@
         <v>13</v>
       </c>
       <c r="F77" s="13" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="G77" s="7" t="s">
         <v>20</v>
@@ -3967,7 +3967,7 @@
         <v>20</v>
       </c>
       <c r="I77" s="13" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="J77" s="7" t="s">
         <v>15</v>
@@ -3981,10 +3981,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="C78" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="D78" t="s">
         <v>22</v>
@@ -3993,7 +3993,7 @@
         <v>13</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="G78" s="7" t="s">
         <v>20</v>
@@ -4014,10 +4014,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="C79" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="D79" t="s">
         <v>22</v>
@@ -4026,7 +4026,7 @@
         <v>13</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="G79" s="7" t="s">
         <v>20</v>
@@ -4047,10 +4047,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="C80" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D80" t="s">
         <v>22</v>
@@ -4059,13 +4059,13 @@
         <v>13</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="G80" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H80" s="7" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="I80" s="7"/>
       <c r="J80" s="7" t="s">
@@ -4080,10 +4080,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="C81" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="D81" t="s">
         <v>22</v>
@@ -4092,13 +4092,13 @@
         <v>13</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="G81" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H81" s="7" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="I81" s="7"/>
       <c r="J81" s="7" t="s">
@@ -4113,10 +4113,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="C82" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="D82" t="s">
         <v>22</v>
@@ -4125,13 +4125,13 @@
         <v>13</v>
       </c>
       <c r="F82" s="7" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="G82" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H82" s="7" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="I82" s="7"/>
       <c r="J82" s="7" t="s">
@@ -4146,10 +4146,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C83" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="D83" t="s">
         <v>22</v>
@@ -4158,13 +4158,13 @@
         <v>13</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="G83" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H83" s="7" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="I83" s="7"/>
       <c r="J83" s="7" t="s">
@@ -4179,10 +4179,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C84" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="D84" t="s">
         <v>22</v>
@@ -4191,13 +4191,13 @@
         <v>13</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="G84" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H84" s="7" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="I84" s="7"/>
       <c r="J84" s="7" t="s">
@@ -4212,10 +4212,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="C85" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="D85" t="s">
         <v>22</v>
@@ -4224,13 +4224,13 @@
         <v>13</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="G85" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H85" s="7" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="I85" s="7"/>
       <c r="J85" s="7" t="s">
@@ -4245,10 +4245,10 @@
         <v>85</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="C86" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="D86" t="s">
         <v>22</v>
@@ -4257,13 +4257,13 @@
         <v>13</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="G86" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H86" s="7" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="I86" s="7"/>
       <c r="J86" s="7" t="s">
@@ -4278,10 +4278,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="C87" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="D87" t="s">
         <v>22</v>
@@ -4290,13 +4290,13 @@
         <v>13</v>
       </c>
       <c r="F87" s="7" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="G87" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="I87" s="7"/>
       <c r="J87" s="7" t="s">
@@ -4311,10 +4311,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="C88" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="D88" t="s">
         <v>22</v>
@@ -4342,10 +4342,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="C89" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="D89" t="s">
         <v>22</v>
@@ -4373,10 +4373,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="C90" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="D90" t="s">
         <v>22</v>
@@ -4404,10 +4404,10 @@
         <v>90</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="C91" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="D91" t="s">
         <v>22</v>
@@ -4416,13 +4416,13 @@
         <v>13</v>
       </c>
       <c r="F91" s="7" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="G91" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H91" s="7" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="I91" s="7"/>
       <c r="J91" s="7" t="s">
@@ -4437,10 +4437,10 @@
         <v>91</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="C92" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="D92" t="s">
         <v>22</v>
@@ -4449,13 +4449,13 @@
         <v>13</v>
       </c>
       <c r="F92" s="7" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="G92" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H92" s="7" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="I92" s="7"/>
       <c r="J92" s="7" t="s">
@@ -4470,10 +4470,10 @@
         <v>92</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="C93" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="D93" t="s">
         <v>22</v>
@@ -4482,7 +4482,7 @@
         <v>13</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>20</v>
@@ -4491,7 +4491,7 @@
         <v>20</v>
       </c>
       <c r="I93" s="7" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="J93" s="7" t="s">
         <v>15</v>
@@ -4505,19 +4505,19 @@
         <v>93</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="C94" t="s">
+        <v>306</v>
+      </c>
+      <c r="D94" t="s">
+        <v>22</v>
+      </c>
+      <c r="E94" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F94" s="1" t="s">
         <v>317</v>
-      </c>
-      <c r="D94" t="s">
-        <v>22</v>
-      </c>
-      <c r="E94" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>328</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>20</v>
@@ -4526,7 +4526,7 @@
         <v>20</v>
       </c>
       <c r="I94" s="7" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="J94" s="7" t="s">
         <v>15</v>
@@ -4540,10 +4540,10 @@
         <v>94</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="C95" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="D95" t="s">
         <v>22</v>
@@ -4552,13 +4552,13 @@
         <v>13</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="G95" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H95" s="7" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="I95" s="7"/>
       <c r="J95" s="7" t="s">
@@ -4573,10 +4573,10 @@
         <v>95</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="C96" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="D96" t="s">
         <v>22</v>
@@ -4585,13 +4585,13 @@
         <v>13</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="G96" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H96" s="7" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="I96" s="7"/>
       <c r="J96" s="7" t="s">
@@ -4606,10 +4606,10 @@
         <v>96</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="C97" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="D97" t="s">
         <v>22</v>
@@ -4618,13 +4618,13 @@
         <v>13</v>
       </c>
       <c r="F97" s="15" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="G97" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H97" s="15" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="I97" s="7"/>
       <c r="J97" s="7" t="s">
@@ -4639,10 +4639,10 @@
         <v>97</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="C98" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="D98" t="s">
         <v>22</v>
@@ -4651,13 +4651,13 @@
         <v>13</v>
       </c>
       <c r="F98" s="15" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="G98" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H98" s="15" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="I98" s="7"/>
       <c r="J98" s="7" t="s">
@@ -4672,10 +4672,10 @@
         <v>98</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="C99" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="D99" t="s">
         <v>22</v>
@@ -4684,13 +4684,13 @@
         <v>13</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="G99" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H99" s="7" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="I99" s="7"/>
       <c r="J99" s="7" t="s">
@@ -4705,10 +4705,10 @@
         <v>99</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="C100" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="D100" t="s">
         <v>22</v>
@@ -4717,13 +4717,13 @@
         <v>13</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="G100" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="I100" s="7"/>
       <c r="J100" s="7" t="s">
@@ -4738,10 +4738,10 @@
         <v>100</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="C101" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="D101" t="s">
         <v>22</v>
@@ -4769,10 +4769,10 @@
         <v>101</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="C102" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="D102" t="s">
         <v>22</v>
@@ -4781,13 +4781,13 @@
         <v>13</v>
       </c>
       <c r="F102" s="7" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="G102" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H102" s="7" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="I102" s="7"/>
       <c r="J102" s="7" t="s">
@@ -4802,10 +4802,10 @@
         <v>102</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="C103" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="D103" t="s">
         <v>22</v>
@@ -4833,10 +4833,10 @@
         <v>103</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="C104" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="D104" t="s">
         <v>22</v>
@@ -4845,13 +4845,13 @@
         <v>13</v>
       </c>
       <c r="F104" s="7" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="G104" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H104" s="15" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="I104" s="7"/>
       <c r="J104" s="7" t="s">
@@ -4866,10 +4866,10 @@
         <v>104</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="C105" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="D105" t="s">
         <v>22</v>
@@ -4878,13 +4878,13 @@
         <v>13</v>
       </c>
       <c r="F105" s="15" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="G105" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H105" s="7" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="I105" s="7"/>
       <c r="J105" s="7" t="s">
@@ -4899,10 +4899,10 @@
         <v>105</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="C106" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="D106" t="s">
         <v>22</v>
@@ -4911,13 +4911,13 @@
         <v>13</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="G106" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H106" s="7" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="I106" s="7"/>
       <c r="J106" s="7" t="s">
@@ -4932,10 +4932,10 @@
         <v>106</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="C107" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="D107" t="s">
         <v>22</v>
@@ -4963,10 +4963,10 @@
         <v>107</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="C108" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="D108" t="s">
         <v>22</v>
@@ -4975,7 +4975,7 @@
         <v>13</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="G108" s="7" t="s">
         <v>20</v>
@@ -4996,10 +4996,10 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="C109" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="D109" t="s">
         <v>12</v>
@@ -5008,16 +5008,16 @@
         <v>13</v>
       </c>
       <c r="F109" s="23" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="H109">
         <v>1</v>
       </c>
       <c r="I109" s="24" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="J109" s="12" t="s">
         <v>15</v>
@@ -5099,6 +5099,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -5339,18 +5351,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5361,6 +5361,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF2265-5030-4B54-A34F-4798AFD4DA4C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2AE2FD3-517E-4530-8BC5-1FF35C67F615}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5379,17 +5390,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF2265-5030-4B54-A34F-4798AFD4DA4C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{398CA3EE-638E-435F-8CA6-D67A7B863103}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
GINI_P2-TOT_PA_QX changed from impossible to operation. FAM1_DIAB2- Algorithm changed LISA_P2-FAM1_DIAB2 algorithm changed
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_GINI_P2.xlsx
+++ b/rmonize/data_proc_elem/DPE_GINI_P2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52413BDC-9100-4D8F-9686-E4AF9739279C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757AC956-946E-48C2-8F3C-2058295C09DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22050" windowHeight="8100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -311,12 +311,6 @@
   </si>
   <si>
     <t>diabmut_15;diabvat_15</t>
-  </si>
-  <si>
-    <t>If either parent has diabetes, the family history is marked as 1.
-If both parents do not have diabetes, the family history is marked as 0.
-If one parent's status is missing or unknown (NA or 3), use the other parent’s status. If the known parent has diabetes, the family history is marked as 1, and if the known parent does not have diabetes, the family history is marked as NA.
-If both parents' statuses are missing -&gt; "" or unknown -&gt; 888, the family history is marked as NA (insufficient data).</t>
   </si>
   <si>
     <t>FAM1_CANCER</t>
@@ -894,16 +888,6 @@
     )</t>
   </si>
   <si>
-    <t>case_when (
-  diabmut_15 == 1 | diabvat_15 == 1 ~ 1L,
-  diabmut_15 == 0 &amp; diabvat_15 == 0 ~ 0L,
-  (is.na(diabmut_15) | diabmut_15 == 3) &amp; diabvat_15 == 0 ~ NA_integer_,
-  (is.na(diabvat_15) | diabvat_15 == 3) &amp; diabmut_15 == 0 ~ NA_integer_,
-  (is.na(diabmut_15) | diabmut_15 == 3) &amp; (is.na(diabvat_15) | diabvat_15 == 3) ~ NA_integer_, 
-  TRUE ~ NA_integer_
-)</t>
-  </si>
-  <si>
     <t>FFQAPFEL_15; FFQBEERE_15; FFQSUED_15; FFQNUSS_15</t>
   </si>
   <si>
@@ -1105,6 +1089,21 @@
   </si>
   <si>
     <t>Age at time of death [years]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If either parent has diabetes, the family history is marked as 1.
+If both parents do not have diabetes, the family history is marked as 0.                                                                                                                       If one parent's status is no or unknown (NA or 3), the family history is marked as 2. 
+If one parent's status is missing or unknown (NA or 3), the family history is marked as 2. </t>
+  </si>
+  <si>
+    <t>case_when (
+  diabmut_15 == 1 | diabvat_15 == 1 ~ 1L,
+  diabmut_15 == 0 &amp; diabvat_15 == 0 ~ 0L,
+   diabmut_15 == 3 &amp; diabvat_15 == 0 ~ 2,
+  diabvat_15 == 3 &amp; diabmut_15 == 0 ~ 2,
+  (is.na(diabmut_15)  &amp;  diabvat_15 == 3 ~ 2,                                                                          (is.na(diabvat_15)  &amp;  diabmut_15 == 3 ~ 2, 
+  TRUE ~ NA_integer_
+)</t>
   </si>
 </sst>
 </file>
@@ -1589,8 +1588,8 @@
   <dimension ref="A1:M131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C109"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,7 +1607,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -1715,7 +1714,7 @@
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D4" t="s">
         <v>22</v>
@@ -1763,7 +1762,7 @@
         <v>27</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>28</v>
@@ -1798,7 +1797,7 @@
         <v>27</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I6" s="16" t="s">
         <v>34</v>
@@ -1847,7 +1846,7 @@
       </c>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1855,7 +1854,7 @@
         <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
@@ -1863,20 +1862,23 @@
       <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="F8" s="20" t="s">
+        <v>45</v>
+      </c>
       <c r="G8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1884,7 +1886,7 @@
         <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
@@ -1892,21 +1894,18 @@
       <c r="E9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="20" t="s">
-        <v>45</v>
-      </c>
       <c r="G9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>258</v>
+        <v>42</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="I9" s="13"/>
-      <c r="J9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>47</v>
+      <c r="J9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1932,7 +1931,7 @@
         <v>38</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>29</v>
@@ -1949,7 +1948,7 @@
         <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
@@ -1978,7 +1977,7 @@
         <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D12" t="s">
         <v>22</v>
@@ -2007,7 +2006,7 @@
         <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D13" t="s">
         <v>22</v>
@@ -2051,7 +2050,7 @@
         <v>38</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>57</v>
@@ -2133,7 +2132,7 @@
         <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
@@ -2163,7 +2162,7 @@
         <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
@@ -2192,7 +2191,7 @@
         <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D19" t="s">
         <v>22</v>
@@ -2221,7 +2220,7 @@
         <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -2256,7 +2255,7 @@
         <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D21" t="s">
         <v>22</v>
@@ -2291,7 +2290,7 @@
         <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D22" t="s">
         <v>22</v>
@@ -2326,7 +2325,7 @@
         <v>74</v>
       </c>
       <c r="C23" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D23" t="s">
         <v>22</v>
@@ -2463,7 +2462,7 @@
         <v>38</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>15</v>
@@ -2527,10 +2526,10 @@
         <v>27</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>264</v>
+        <v>328</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>90</v>
+        <v>327</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>29</v>
@@ -2545,10 +2544,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" t="s">
         <v>91</v>
-      </c>
-      <c r="C30" t="s">
-        <v>92</v>
       </c>
       <c r="D30" t="s">
         <v>12</v>
@@ -2575,10 +2574,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" t="s">
         <v>93</v>
-      </c>
-      <c r="C31" t="s">
-        <v>94</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
@@ -2604,10 +2603,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" t="s">
         <v>95</v>
-      </c>
-      <c r="C32" t="s">
-        <v>96</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
@@ -2633,10 +2632,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" t="s">
         <v>97</v>
-      </c>
-      <c r="C33" t="s">
-        <v>98</v>
       </c>
       <c r="D33" t="s">
         <v>12</v>
@@ -2662,10 +2661,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" t="s">
         <v>99</v>
-      </c>
-      <c r="C34" t="s">
-        <v>100</v>
       </c>
       <c r="D34" t="s">
         <v>12</v>
@@ -2691,10 +2690,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C35" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D35" t="s">
         <v>12</v>
@@ -2720,10 +2719,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C36" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D36" t="s">
         <v>12</v>
@@ -2749,10 +2748,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C37" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D37" t="s">
         <v>12</v>
@@ -2778,10 +2777,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" t="s">
         <v>104</v>
-      </c>
-      <c r="C38" t="s">
-        <v>105</v>
       </c>
       <c r="D38" t="s">
         <v>12</v>
@@ -2807,10 +2806,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" t="s">
         <v>106</v>
-      </c>
-      <c r="C39" t="s">
-        <v>107</v>
       </c>
       <c r="D39" t="s">
         <v>12</v>
@@ -2836,10 +2835,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" t="s">
         <v>108</v>
-      </c>
-      <c r="C40" t="s">
-        <v>109</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
@@ -2865,10 +2864,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C41" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D41" t="s">
         <v>22</v>
@@ -2894,10 +2893,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" t="s">
         <v>111</v>
-      </c>
-      <c r="C42" t="s">
-        <v>112</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
@@ -2923,10 +2922,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C43" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D43" t="s">
         <v>22</v>
@@ -2952,10 +2951,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" t="s">
         <v>114</v>
-      </c>
-      <c r="C44" t="s">
-        <v>115</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
@@ -2981,10 +2980,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C45" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D45" t="s">
         <v>22</v>
@@ -3010,10 +3009,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C46" t="s">
         <v>117</v>
-      </c>
-      <c r="C46" t="s">
-        <v>118</v>
       </c>
       <c r="D46" t="s">
         <v>12</v>
@@ -3039,10 +3038,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C47" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D47" t="s">
         <v>22</v>
@@ -3068,10 +3067,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C48" t="s">
         <v>120</v>
-      </c>
-      <c r="C48" t="s">
-        <v>121</v>
       </c>
       <c r="D48" t="s">
         <v>12</v>
@@ -3097,10 +3096,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C49" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D49" t="s">
         <v>22</v>
@@ -3126,10 +3125,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C50" t="s">
         <v>123</v>
-      </c>
-      <c r="C50" t="s">
-        <v>124</v>
       </c>
       <c r="D50" t="s">
         <v>12</v>
@@ -3155,10 +3154,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C51" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D51" t="s">
         <v>22</v>
@@ -3184,10 +3183,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C52" t="s">
         <v>126</v>
-      </c>
-      <c r="C52" t="s">
-        <v>127</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
@@ -3213,10 +3212,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C53" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D53" t="s">
         <v>22</v>
@@ -3242,10 +3241,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C54" t="s">
         <v>129</v>
-      </c>
-      <c r="C54" t="s">
-        <v>130</v>
       </c>
       <c r="D54" t="s">
         <v>12</v>
@@ -3271,10 +3270,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C55" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D55" t="s">
         <v>22</v>
@@ -3300,10 +3299,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
+        <v>131</v>
+      </c>
+      <c r="C56" t="s">
         <v>132</v>
-      </c>
-      <c r="C56" t="s">
-        <v>133</v>
       </c>
       <c r="D56" t="s">
         <v>12</v>
@@ -3329,10 +3328,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C57" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D57" t="s">
         <v>22</v>
@@ -3358,10 +3357,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C58" t="s">
         <v>135</v>
-      </c>
-      <c r="C58" t="s">
-        <v>136</v>
       </c>
       <c r="D58" t="s">
         <v>12</v>
@@ -3388,13 +3387,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C59" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D59" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>13</v>
@@ -3417,19 +3416,19 @@
         <v>59</v>
       </c>
       <c r="B60" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C60" t="s">
+        <v>325</v>
+      </c>
+      <c r="D60" t="s">
+        <v>22</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F60" s="4" t="s">
         <v>138</v>
-      </c>
-      <c r="C60" t="s">
-        <v>327</v>
-      </c>
-      <c r="D60" t="s">
-        <v>22</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>139</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>20</v>
@@ -3449,10 +3448,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C61" t="s">
         <v>140</v>
-      </c>
-      <c r="C61" t="s">
-        <v>141</v>
       </c>
       <c r="D61" t="s">
         <v>12</v>
@@ -3478,10 +3477,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C62" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D62" t="s">
         <v>22</v>
@@ -3507,10 +3506,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C63" t="s">
         <v>143</v>
-      </c>
-      <c r="C63" t="s">
-        <v>144</v>
       </c>
       <c r="D63" t="s">
         <v>12</v>
@@ -3536,10 +3535,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C64" t="s">
         <v>145</v>
-      </c>
-      <c r="C64" t="s">
-        <v>146</v>
       </c>
       <c r="D64" t="s">
         <v>12</v>
@@ -3565,19 +3564,19 @@
         <v>64</v>
       </c>
       <c r="B65" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C65" t="s">
+        <v>290</v>
+      </c>
+      <c r="D65" t="s">
+        <v>22</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="7" t="s">
         <v>147</v>
-      </c>
-      <c r="C65" t="s">
-        <v>292</v>
-      </c>
-      <c r="D65" t="s">
-        <v>22</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F65" s="7" t="s">
-        <v>148</v>
       </c>
       <c r="G65" s="7" t="s">
         <v>20</v>
@@ -3597,10 +3596,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C66" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D66" t="s">
         <v>22</v>
@@ -3609,7 +3608,7 @@
         <v>13</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G66" s="7" t="s">
         <v>20</v>
@@ -3630,10 +3629,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C67" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D67" t="s">
         <v>22</v>
@@ -3642,7 +3641,7 @@
         <v>13</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G67" s="7" t="s">
         <v>20</v>
@@ -3663,10 +3662,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C68" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D68" t="s">
         <v>22</v>
@@ -3675,7 +3674,7 @@
         <v>13</v>
       </c>
       <c r="F68" s="15" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G68" s="7" t="s">
         <v>20</v>
@@ -3696,10 +3695,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C69" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D69" t="s">
         <v>22</v>
@@ -3727,10 +3726,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C70" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D70" t="s">
         <v>22</v>
@@ -3758,10 +3757,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C71" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D71" t="s">
         <v>22</v>
@@ -3789,10 +3788,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C72" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D72" t="s">
         <v>22</v>
@@ -3820,10 +3819,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C73" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D73" t="s">
         <v>22</v>
@@ -3851,10 +3850,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C74" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D74" t="s">
         <v>22</v>
@@ -3882,10 +3881,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C75" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D75" t="s">
         <v>22</v>
@@ -3894,7 +3893,7 @@
         <v>13</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G75" s="7" t="s">
         <v>20</v>
@@ -3915,10 +3914,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C76" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D76" t="s">
         <v>22</v>
@@ -3946,19 +3945,19 @@
         <v>76</v>
       </c>
       <c r="B77" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C77" t="s">
+        <v>302</v>
+      </c>
+      <c r="D77" t="s">
+        <v>22</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F77" s="13" t="s">
         <v>160</v>
-      </c>
-      <c r="C77" t="s">
-        <v>304</v>
-      </c>
-      <c r="D77" t="s">
-        <v>22</v>
-      </c>
-      <c r="E77" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F77" s="13" t="s">
-        <v>161</v>
       </c>
       <c r="G77" s="7" t="s">
         <v>20</v>
@@ -3967,7 +3966,7 @@
         <v>20</v>
       </c>
       <c r="I77" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J77" s="7" t="s">
         <v>15</v>
@@ -3981,10 +3980,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C78" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D78" t="s">
         <v>22</v>
@@ -3993,7 +3992,7 @@
         <v>13</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G78" s="7" t="s">
         <v>20</v>
@@ -4014,19 +4013,19 @@
         <v>78</v>
       </c>
       <c r="B79" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C79" t="s">
         <v>164</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
+        <v>22</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F79" s="7" t="s">
         <v>165</v>
-      </c>
-      <c r="D79" t="s">
-        <v>22</v>
-      </c>
-      <c r="E79" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>166</v>
       </c>
       <c r="G79" s="7" t="s">
         <v>20</v>
@@ -4047,25 +4046,25 @@
         <v>79</v>
       </c>
       <c r="B80" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C80" t="s">
         <v>167</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D80" t="s">
+        <v>22</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F80" s="7" t="s">
         <v>168</v>
-      </c>
-      <c r="D80" t="s">
-        <v>22</v>
-      </c>
-      <c r="E80" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F80" s="7" t="s">
-        <v>169</v>
       </c>
       <c r="G80" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H80" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I80" s="7"/>
       <c r="J80" s="7" t="s">
@@ -4080,25 +4079,25 @@
         <v>80</v>
       </c>
       <c r="B81" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C81" t="s">
         <v>171</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
+        <v>22</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F81" s="7" t="s">
         <v>172</v>
-      </c>
-      <c r="D81" t="s">
-        <v>22</v>
-      </c>
-      <c r="E81" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F81" s="7" t="s">
-        <v>173</v>
       </c>
       <c r="G81" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H81" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I81" s="7"/>
       <c r="J81" s="7" t="s">
@@ -4113,25 +4112,25 @@
         <v>81</v>
       </c>
       <c r="B82" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C82" t="s">
         <v>175</v>
       </c>
-      <c r="C82" t="s">
+      <c r="D82" t="s">
+        <v>22</v>
+      </c>
+      <c r="E82" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F82" s="7" t="s">
         <v>176</v>
-      </c>
-      <c r="D82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E82" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F82" s="7" t="s">
-        <v>177</v>
       </c>
       <c r="G82" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H82" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I82" s="7"/>
       <c r="J82" s="7" t="s">
@@ -4146,25 +4145,25 @@
         <v>82</v>
       </c>
       <c r="B83" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C83" t="s">
         <v>179</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
+        <v>22</v>
+      </c>
+      <c r="E83" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F83" s="7" t="s">
         <v>180</v>
-      </c>
-      <c r="D83" t="s">
-        <v>22</v>
-      </c>
-      <c r="E83" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F83" s="7" t="s">
-        <v>181</v>
       </c>
       <c r="G83" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H83" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I83" s="7"/>
       <c r="J83" s="7" t="s">
@@ -4179,25 +4178,25 @@
         <v>83</v>
       </c>
       <c r="B84" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C84" t="s">
         <v>183</v>
       </c>
-      <c r="C84" t="s">
+      <c r="D84" t="s">
+        <v>22</v>
+      </c>
+      <c r="E84" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F84" s="7" t="s">
         <v>184</v>
-      </c>
-      <c r="D84" t="s">
-        <v>22</v>
-      </c>
-      <c r="E84" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F84" s="7" t="s">
-        <v>185</v>
       </c>
       <c r="G84" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H84" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I84" s="7"/>
       <c r="J84" s="7" t="s">
@@ -4212,25 +4211,25 @@
         <v>84</v>
       </c>
       <c r="B85" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C85" t="s">
         <v>187</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D85" t="s">
+        <v>22</v>
+      </c>
+      <c r="E85" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F85" s="7" t="s">
         <v>188</v>
-      </c>
-      <c r="D85" t="s">
-        <v>22</v>
-      </c>
-      <c r="E85" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F85" s="7" t="s">
-        <v>189</v>
       </c>
       <c r="G85" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H85" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I85" s="7"/>
       <c r="J85" s="7" t="s">
@@ -4245,25 +4244,25 @@
         <v>85</v>
       </c>
       <c r="B86" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C86" t="s">
         <v>191</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
+        <v>22</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F86" s="7" t="s">
         <v>192</v>
-      </c>
-      <c r="D86" t="s">
-        <v>22</v>
-      </c>
-      <c r="E86" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F86" s="7" t="s">
-        <v>193</v>
       </c>
       <c r="G86" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H86" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I86" s="7"/>
       <c r="J86" s="7" t="s">
@@ -4278,25 +4277,25 @@
         <v>86</v>
       </c>
       <c r="B87" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C87" t="s">
         <v>195</v>
       </c>
-      <c r="C87" t="s">
+      <c r="D87" t="s">
+        <v>22</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F87" s="7" t="s">
         <v>196</v>
-      </c>
-      <c r="D87" t="s">
-        <v>22</v>
-      </c>
-      <c r="E87" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F87" s="7" t="s">
-        <v>197</v>
       </c>
       <c r="G87" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I87" s="7"/>
       <c r="J87" s="7" t="s">
@@ -4311,10 +4310,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C88" t="s">
         <v>199</v>
-      </c>
-      <c r="C88" t="s">
-        <v>200</v>
       </c>
       <c r="D88" t="s">
         <v>22</v>
@@ -4342,10 +4341,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C89" t="s">
         <v>201</v>
-      </c>
-      <c r="C89" t="s">
-        <v>202</v>
       </c>
       <c r="D89" t="s">
         <v>22</v>
@@ -4373,10 +4372,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C90" t="s">
         <v>203</v>
-      </c>
-      <c r="C90" t="s">
-        <v>204</v>
       </c>
       <c r="D90" t="s">
         <v>22</v>
@@ -4404,25 +4403,25 @@
         <v>90</v>
       </c>
       <c r="B91" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C91" t="s">
         <v>205</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F91" s="7" t="s">
         <v>206</v>
-      </c>
-      <c r="D91" t="s">
-        <v>22</v>
-      </c>
-      <c r="E91" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F91" s="7" t="s">
-        <v>207</v>
       </c>
       <c r="G91" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H91" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I91" s="7"/>
       <c r="J91" s="7" t="s">
@@ -4437,25 +4436,25 @@
         <v>91</v>
       </c>
       <c r="B92" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C92" t="s">
         <v>209</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D92" t="s">
+        <v>22</v>
+      </c>
+      <c r="E92" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F92" s="7" t="s">
         <v>210</v>
-      </c>
-      <c r="D92" t="s">
-        <v>22</v>
-      </c>
-      <c r="E92" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F92" s="7" t="s">
-        <v>211</v>
       </c>
       <c r="G92" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H92" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I92" s="7"/>
       <c r="J92" s="7" t="s">
@@ -4470,11 +4469,11 @@
         <v>92</v>
       </c>
       <c r="B93" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C93" t="s">
         <v>213</v>
       </c>
-      <c r="C93" t="s">
-        <v>214</v>
-      </c>
       <c r="D93" t="s">
         <v>22</v>
       </c>
@@ -4482,7 +4481,7 @@
         <v>13</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>20</v>
@@ -4491,7 +4490,7 @@
         <v>20</v>
       </c>
       <c r="I93" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J93" s="7" t="s">
         <v>15</v>
@@ -4505,10 +4504,10 @@
         <v>93</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C94" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D94" t="s">
         <v>22</v>
@@ -4517,7 +4516,7 @@
         <v>13</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>20</v>
@@ -4526,7 +4525,7 @@
         <v>20</v>
       </c>
       <c r="I94" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J94" s="7" t="s">
         <v>15</v>
@@ -4540,25 +4539,25 @@
         <v>94</v>
       </c>
       <c r="B95" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C95" t="s">
         <v>217</v>
       </c>
-      <c r="C95" t="s">
+      <c r="D95" t="s">
+        <v>22</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F95" s="7" t="s">
         <v>218</v>
-      </c>
-      <c r="D95" t="s">
-        <v>22</v>
-      </c>
-      <c r="E95" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F95" s="7" t="s">
-        <v>219</v>
       </c>
       <c r="G95" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H95" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I95" s="7"/>
       <c r="J95" s="7" t="s">
@@ -4573,25 +4572,25 @@
         <v>95</v>
       </c>
       <c r="B96" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C96" t="s">
         <v>221</v>
       </c>
-      <c r="C96" t="s">
+      <c r="D96" t="s">
+        <v>22</v>
+      </c>
+      <c r="E96" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F96" s="7" t="s">
         <v>222</v>
-      </c>
-      <c r="D96" t="s">
-        <v>22</v>
-      </c>
-      <c r="E96" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F96" s="7" t="s">
-        <v>223</v>
       </c>
       <c r="G96" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H96" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I96" s="7"/>
       <c r="J96" s="7" t="s">
@@ -4606,11 +4605,11 @@
         <v>96</v>
       </c>
       <c r="B97" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C97" t="s">
         <v>225</v>
       </c>
-      <c r="C97" t="s">
-        <v>226</v>
-      </c>
       <c r="D97" t="s">
         <v>22</v>
       </c>
@@ -4618,13 +4617,13 @@
         <v>13</v>
       </c>
       <c r="F97" s="15" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G97" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H97" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I97" s="7"/>
       <c r="J97" s="7" t="s">
@@ -4639,10 +4638,10 @@
         <v>97</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C98" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D98" t="s">
         <v>22</v>
@@ -4651,13 +4650,13 @@
         <v>13</v>
       </c>
       <c r="F98" s="15" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G98" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H98" s="15" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I98" s="7"/>
       <c r="J98" s="7" t="s">
@@ -4672,25 +4671,25 @@
         <v>98</v>
       </c>
       <c r="B99" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C99" t="s">
+        <v>306</v>
+      </c>
+      <c r="D99" t="s">
+        <v>22</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F99" s="7" t="s">
         <v>229</v>
-      </c>
-      <c r="C99" t="s">
-        <v>308</v>
-      </c>
-      <c r="D99" t="s">
-        <v>22</v>
-      </c>
-      <c r="E99" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F99" s="7" t="s">
-        <v>230</v>
       </c>
       <c r="G99" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H99" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I99" s="7"/>
       <c r="J99" s="7" t="s">
@@ -4705,25 +4704,25 @@
         <v>99</v>
       </c>
       <c r="B100" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C100" t="s">
+        <v>307</v>
+      </c>
+      <c r="D100" t="s">
+        <v>22</v>
+      </c>
+      <c r="E100" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F100" s="7" t="s">
         <v>232</v>
-      </c>
-      <c r="C100" t="s">
-        <v>309</v>
-      </c>
-      <c r="D100" t="s">
-        <v>22</v>
-      </c>
-      <c r="E100" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F100" s="7" t="s">
-        <v>233</v>
       </c>
       <c r="G100" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I100" s="7"/>
       <c r="J100" s="7" t="s">
@@ -4738,10 +4737,10 @@
         <v>100</v>
       </c>
       <c r="B101" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C101" t="s">
         <v>235</v>
-      </c>
-      <c r="C101" t="s">
-        <v>236</v>
       </c>
       <c r="D101" t="s">
         <v>22</v>
@@ -4769,25 +4768,25 @@
         <v>101</v>
       </c>
       <c r="B102" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="C102" t="s">
         <v>237</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D102" t="s">
+        <v>22</v>
+      </c>
+      <c r="E102" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F102" s="7" t="s">
         <v>238</v>
-      </c>
-      <c r="D102" t="s">
-        <v>22</v>
-      </c>
-      <c r="E102" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F102" s="7" t="s">
-        <v>239</v>
       </c>
       <c r="G102" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H102" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I102" s="7"/>
       <c r="J102" s="7" t="s">
@@ -4802,10 +4801,10 @@
         <v>102</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C103" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D103" t="s">
         <v>22</v>
@@ -4833,10 +4832,10 @@
         <v>103</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C104" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D104" t="s">
         <v>22</v>
@@ -4845,13 +4844,13 @@
         <v>13</v>
       </c>
       <c r="F104" s="7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G104" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H104" s="15" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I104" s="7"/>
       <c r="J104" s="7" t="s">
@@ -4866,11 +4865,11 @@
         <v>104</v>
       </c>
       <c r="B105" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="C105" t="s">
         <v>243</v>
       </c>
-      <c r="C105" t="s">
-        <v>244</v>
-      </c>
       <c r="D105" t="s">
         <v>22</v>
       </c>
@@ -4878,13 +4877,13 @@
         <v>13</v>
       </c>
       <c r="F105" s="15" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G105" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H105" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="I105" s="7"/>
       <c r="J105" s="7" t="s">
@@ -4899,25 +4898,25 @@
         <v>105</v>
       </c>
       <c r="B106" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C106" t="s">
         <v>245</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D106" t="s">
+        <v>22</v>
+      </c>
+      <c r="E106" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F106" s="7" t="s">
         <v>246</v>
-      </c>
-      <c r="D106" t="s">
-        <v>22</v>
-      </c>
-      <c r="E106" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F106" s="7" t="s">
-        <v>247</v>
       </c>
       <c r="G106" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H106" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I106" s="7"/>
       <c r="J106" s="7" t="s">
@@ -4932,10 +4931,10 @@
         <v>106</v>
       </c>
       <c r="B107" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="C107" t="s">
         <v>249</v>
-      </c>
-      <c r="C107" t="s">
-        <v>250</v>
       </c>
       <c r="D107" t="s">
         <v>22</v>
@@ -4963,19 +4962,19 @@
         <v>107</v>
       </c>
       <c r="B108" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="C108" t="s">
         <v>251</v>
       </c>
-      <c r="C108" t="s">
+      <c r="D108" t="s">
+        <v>22</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F108" s="7" t="s">
         <v>252</v>
-      </c>
-      <c r="D108" t="s">
-        <v>22</v>
-      </c>
-      <c r="E108" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F108" s="7" t="s">
-        <v>253</v>
       </c>
       <c r="G108" s="7" t="s">
         <v>20</v>
@@ -4996,10 +4995,10 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
+        <v>253</v>
+      </c>
+      <c r="C109" t="s">
         <v>254</v>
-      </c>
-      <c r="C109" t="s">
-        <v>255</v>
       </c>
       <c r="D109" t="s">
         <v>12</v>
@@ -5008,16 +5007,16 @@
         <v>13</v>
       </c>
       <c r="F109" s="23" t="s">
+        <v>255</v>
+      </c>
+      <c r="G109" s="3" t="s">
         <v>256</v>
-      </c>
-      <c r="G109" s="3" t="s">
-        <v>257</v>
       </c>
       <c r="H109">
         <v>1</v>
       </c>
       <c r="I109" s="24" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="J109" s="12" t="s">
         <v>15</v>
@@ -5111,6 +5110,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -5351,15 +5359,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF2265-5030-4B54-A34F-4798AFD4DA4C}">
   <ds:schemaRefs>
@@ -5372,6 +5371,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{398CA3EE-638E-435F-8CA6-D67A7B863103}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2AE2FD3-517E-4530-8BC5-1FF35C67F615}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5388,12 +5395,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{398CA3EE-638E-435F-8CA6-D67A7B863103}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GINI__P2- TOT_PA_QX changed from impossible to operation. GINI__P2-FAM1_DIAB2 algorithm changed LISA_P2-FAM1_DIAB2 algorithm changed
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_GINI_P2.xlsx
+++ b/rmonize/data_proc_elem/DPE_GINI_P2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757AC956-946E-48C2-8F3C-2058295C09DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0EEE453-E4C7-4D0F-9DB0-0F0E957A5BA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22050" windowHeight="8100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1587,9 +1587,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5098,27 +5098,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -5359,26 +5338,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF2265-5030-4B54-A34F-4798AFD4DA4C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{398CA3EE-638E-435F-8CA6-D67A7B863103}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2AE2FD3-517E-4530-8BC5-1FF35C67F615}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5395,4 +5376,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{398CA3EE-638E-435F-8CA6-D67A7B863103}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF2265-5030-4B54-A34F-4798AFD4DA4C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GL-3:Change with the unit for Sodium and NA:K ratio Changed to "direct mapping" for harmo. status for sodium. Changes in the algorithm for family status(addition of L).
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_GINI_P2.xlsx
+++ b/rmonize/data_proc_elem/DPE_GINI_P2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0EEE453-E4C7-4D0F-9DB0-0F0E957A5BA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E838CA-3D7A-4A95-97D3-6DB7462FD167}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22050" windowHeight="8100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="328">
   <si>
     <t>dataschema_variable</t>
   </si>
@@ -694,19 +694,10 @@
     <t>SODIUM</t>
   </si>
   <si>
-    <t>Sodium intake [g/d]</t>
-  </si>
-  <si>
     <t xml:space="preserve">FFQMNA_15 </t>
   </si>
   <si>
-    <t>FFQMNA_15 /1000</t>
-  </si>
-  <si>
     <t>SOD_POT_RATIO</t>
-  </si>
-  <si>
-    <t>Sodium to potassium intake ratio [g/d]</t>
   </si>
   <si>
     <t>FFQMK_15; FFQMNA_15</t>
@@ -1099,11 +1090,17 @@
     <t>case_when (
   diabmut_15 == 1 | diabvat_15 == 1 ~ 1L,
   diabmut_15 == 0 &amp; diabvat_15 == 0 ~ 0L,
-   diabmut_15 == 3 &amp; diabvat_15 == 0 ~ 2,
-  diabvat_15 == 3 &amp; diabmut_15 == 0 ~ 2,
-  (is.na(diabmut_15)  &amp;  diabvat_15 == 3 ~ 2,                                                                          (is.na(diabvat_15)  &amp;  diabmut_15 == 3 ~ 2, 
+   diabmut_15 == 3 &amp; diabvat_15 == 0 ~ 2L,
+  diabvat_15 == 3 &amp; diabmut_15 == 0 ~ 2L,
+  (is.na(diabmut_15)  &amp;  diabvat_15 == 3 ~ 2L,                                                                          (is.na(diabvat_15)  &amp;  diabmut_15 == 3 ~ 2L, 
   TRUE ~ NA_integer_
 )</t>
+  </si>
+  <si>
+    <t>Sodium intake [mg/d]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sodium to potassium intake ratio </t>
   </si>
 </sst>
 </file>
@@ -1587,9 +1584,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,7 +1604,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -1714,7 +1711,7 @@
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D4" t="s">
         <v>22</v>
@@ -1762,7 +1759,7 @@
         <v>27</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>28</v>
@@ -1797,7 +1794,7 @@
         <v>27</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="I6" s="16" t="s">
         <v>34</v>
@@ -1854,7 +1851,7 @@
         <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
@@ -1869,7 +1866,7 @@
         <v>46</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>15</v>
@@ -1886,7 +1883,7 @@
         <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
@@ -1931,7 +1928,7 @@
         <v>38</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>29</v>
@@ -1948,7 +1945,7 @@
         <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
@@ -1977,7 +1974,7 @@
         <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D12" t="s">
         <v>22</v>
@@ -2006,7 +2003,7 @@
         <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D13" t="s">
         <v>22</v>
@@ -2050,7 +2047,7 @@
         <v>38</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>57</v>
@@ -2132,7 +2129,7 @@
         <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
@@ -2162,7 +2159,7 @@
         <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
@@ -2191,7 +2188,7 @@
         <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D19" t="s">
         <v>22</v>
@@ -2220,7 +2217,7 @@
         <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -2255,7 +2252,7 @@
         <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D21" t="s">
         <v>22</v>
@@ -2290,7 +2287,7 @@
         <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D22" t="s">
         <v>22</v>
@@ -2325,7 +2322,7 @@
         <v>74</v>
       </c>
       <c r="C23" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D23" t="s">
         <v>22</v>
@@ -2462,7 +2459,7 @@
         <v>38</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>15</v>
@@ -2526,10 +2523,10 @@
         <v>27</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>29</v>
@@ -2693,7 +2690,7 @@
         <v>100</v>
       </c>
       <c r="C35" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D35" t="s">
         <v>12</v>
@@ -2722,7 +2719,7 @@
         <v>101</v>
       </c>
       <c r="C36" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D36" t="s">
         <v>12</v>
@@ -2751,7 +2748,7 @@
         <v>102</v>
       </c>
       <c r="C37" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D37" t="s">
         <v>12</v>
@@ -2867,7 +2864,7 @@
         <v>109</v>
       </c>
       <c r="C41" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D41" t="s">
         <v>22</v>
@@ -2925,7 +2922,7 @@
         <v>112</v>
       </c>
       <c r="C43" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D43" t="s">
         <v>22</v>
@@ -2983,7 +2980,7 @@
         <v>115</v>
       </c>
       <c r="C45" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D45" t="s">
         <v>22</v>
@@ -3041,7 +3038,7 @@
         <v>118</v>
       </c>
       <c r="C47" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D47" t="s">
         <v>22</v>
@@ -3099,7 +3096,7 @@
         <v>121</v>
       </c>
       <c r="C49" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D49" t="s">
         <v>22</v>
@@ -3157,7 +3154,7 @@
         <v>124</v>
       </c>
       <c r="C51" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D51" t="s">
         <v>22</v>
@@ -3215,7 +3212,7 @@
         <v>127</v>
       </c>
       <c r="C53" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D53" t="s">
         <v>22</v>
@@ -3273,7 +3270,7 @@
         <v>130</v>
       </c>
       <c r="C55" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D55" t="s">
         <v>22</v>
@@ -3331,7 +3328,7 @@
         <v>133</v>
       </c>
       <c r="C57" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D57" t="s">
         <v>22</v>
@@ -3390,10 +3387,10 @@
         <v>136</v>
       </c>
       <c r="C59" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D59" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>13</v>
@@ -3419,7 +3416,7 @@
         <v>137</v>
       </c>
       <c r="C60" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D60" t="s">
         <v>22</v>
@@ -3480,7 +3477,7 @@
         <v>141</v>
       </c>
       <c r="C62" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D62" t="s">
         <v>22</v>
@@ -3567,7 +3564,7 @@
         <v>146</v>
       </c>
       <c r="C65" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D65" t="s">
         <v>22</v>
@@ -3599,7 +3596,7 @@
         <v>148</v>
       </c>
       <c r="C66" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D66" t="s">
         <v>22</v>
@@ -3608,7 +3605,7 @@
         <v>13</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G66" s="7" t="s">
         <v>20</v>
@@ -3632,7 +3629,7 @@
         <v>149</v>
       </c>
       <c r="C67" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D67" t="s">
         <v>22</v>
@@ -3641,7 +3638,7 @@
         <v>13</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="G67" s="7" t="s">
         <v>20</v>
@@ -3665,7 +3662,7 @@
         <v>150</v>
       </c>
       <c r="C68" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D68" t="s">
         <v>22</v>
@@ -3674,7 +3671,7 @@
         <v>13</v>
       </c>
       <c r="F68" s="15" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G68" s="7" t="s">
         <v>20</v>
@@ -3698,7 +3695,7 @@
         <v>151</v>
       </c>
       <c r="C69" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D69" t="s">
         <v>22</v>
@@ -3729,7 +3726,7 @@
         <v>152</v>
       </c>
       <c r="C70" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D70" t="s">
         <v>22</v>
@@ -3760,7 +3757,7 @@
         <v>153</v>
       </c>
       <c r="C71" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D71" t="s">
         <v>22</v>
@@ -3791,7 +3788,7 @@
         <v>154</v>
       </c>
       <c r="C72" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D72" t="s">
         <v>22</v>
@@ -3822,7 +3819,7 @@
         <v>155</v>
       </c>
       <c r="C73" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D73" t="s">
         <v>22</v>
@@ -3853,7 +3850,7 @@
         <v>156</v>
       </c>
       <c r="C74" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D74" t="s">
         <v>22</v>
@@ -3884,7 +3881,7 @@
         <v>157</v>
       </c>
       <c r="C75" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D75" t="s">
         <v>22</v>
@@ -3893,7 +3890,7 @@
         <v>13</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G75" s="7" t="s">
         <v>20</v>
@@ -3917,7 +3914,7 @@
         <v>158</v>
       </c>
       <c r="C76" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D76" t="s">
         <v>22</v>
@@ -3948,7 +3945,7 @@
         <v>159</v>
       </c>
       <c r="C77" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D77" t="s">
         <v>22</v>
@@ -3983,7 +3980,7 @@
         <v>162</v>
       </c>
       <c r="C78" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D78" t="s">
         <v>22</v>
@@ -4481,7 +4478,7 @@
         <v>13</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>20</v>
@@ -4507,7 +4504,7 @@
         <v>215</v>
       </c>
       <c r="C94" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D94" t="s">
         <v>22</v>
@@ -4516,7 +4513,7 @@
         <v>13</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>20</v>
@@ -4542,22 +4539,22 @@
         <v>216</v>
       </c>
       <c r="C95" t="s">
+        <v>326</v>
+      </c>
+      <c r="D95" t="s">
+        <v>22</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F95" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="D95" t="s">
-        <v>22</v>
-      </c>
-      <c r="E95" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F95" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="G95" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H95" s="7" t="s">
-        <v>219</v>
+      <c r="G95" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="I95" s="7"/>
       <c r="J95" s="7" t="s">
@@ -4572,10 +4569,10 @@
         <v>95</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C96" t="s">
-        <v>221</v>
+        <v>327</v>
       </c>
       <c r="D96" t="s">
         <v>22</v>
@@ -4584,13 +4581,13 @@
         <v>13</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G96" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H96" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I96" s="7"/>
       <c r="J96" s="7" t="s">
@@ -4605,10 +4602,10 @@
         <v>96</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C97" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D97" t="s">
         <v>22</v>
@@ -4617,13 +4614,13 @@
         <v>13</v>
       </c>
       <c r="F97" s="15" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G97" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H97" s="15" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="I97" s="7"/>
       <c r="J97" s="7" t="s">
@@ -4638,10 +4635,10 @@
         <v>97</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C98" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D98" t="s">
         <v>22</v>
@@ -4650,13 +4647,13 @@
         <v>13</v>
       </c>
       <c r="F98" s="15" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G98" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H98" s="15" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="I98" s="7"/>
       <c r="J98" s="7" t="s">
@@ -4671,10 +4668,10 @@
         <v>98</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C99" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D99" t="s">
         <v>22</v>
@@ -4683,13 +4680,13 @@
         <v>13</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G99" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H99" s="7" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="I99" s="7"/>
       <c r="J99" s="7" t="s">
@@ -4704,10 +4701,10 @@
         <v>99</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C100" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D100" t="s">
         <v>22</v>
@@ -4716,13 +4713,13 @@
         <v>13</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="G100" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="I100" s="7"/>
       <c r="J100" s="7" t="s">
@@ -4737,10 +4734,10 @@
         <v>100</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C101" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D101" t="s">
         <v>22</v>
@@ -4768,10 +4765,10 @@
         <v>101</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C102" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D102" t="s">
         <v>22</v>
@@ -4780,13 +4777,13 @@
         <v>13</v>
       </c>
       <c r="F102" s="7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G102" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H102" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="I102" s="7"/>
       <c r="J102" s="7" t="s">
@@ -4801,10 +4798,10 @@
         <v>102</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C103" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D103" t="s">
         <v>22</v>
@@ -4832,10 +4829,10 @@
         <v>103</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C104" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D104" t="s">
         <v>22</v>
@@ -4844,13 +4841,13 @@
         <v>13</v>
       </c>
       <c r="F104" s="7" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G104" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H104" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="I104" s="7"/>
       <c r="J104" s="7" t="s">
@@ -4865,10 +4862,10 @@
         <v>104</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C105" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D105" t="s">
         <v>22</v>
@@ -4877,13 +4874,13 @@
         <v>13</v>
       </c>
       <c r="F105" s="15" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G105" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H105" s="7" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I105" s="7"/>
       <c r="J105" s="7" t="s">
@@ -4898,10 +4895,10 @@
         <v>105</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C106" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D106" t="s">
         <v>22</v>
@@ -4910,13 +4907,13 @@
         <v>13</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="G106" s="7" t="s">
         <v>46</v>
       </c>
       <c r="H106" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="I106" s="7"/>
       <c r="J106" s="7" t="s">
@@ -4931,10 +4928,10 @@
         <v>106</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C107" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D107" t="s">
         <v>22</v>
@@ -4962,10 +4959,10 @@
         <v>107</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C108" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D108" t="s">
         <v>22</v>
@@ -4974,7 +4971,7 @@
         <v>13</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G108" s="7" t="s">
         <v>20</v>
@@ -4995,10 +4992,10 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C109" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D109" t="s">
         <v>12</v>
@@ -5007,16 +5004,16 @@
         <v>13</v>
       </c>
       <c r="F109" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="H109">
         <v>1</v>
       </c>
       <c r="I109" s="24" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="J109" s="12" t="s">
         <v>15</v>
@@ -5098,6 +5095,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -5338,28 +5356,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF2265-5030-4B54-A34F-4798AFD4DA4C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{398CA3EE-638E-435F-8CA6-D67A7B863103}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2AE2FD3-517E-4530-8BC5-1FF35C67F615}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5376,23 +5392,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{398CA3EE-638E-435F-8CA6-D67A7B863103}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF2265-5030-4B54-A34F-4798AFD4DA4C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GL-4 DPE_GINI_P2 updated algorithm for FAM1_DIAB2
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_GINI_P2.xlsx
+++ b/rmonize/data_proc_elem/DPE_GINI_P2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E838CA-3D7A-4A95-97D3-6DB7462FD167}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632AF36A-8C99-4887-8FCF-B7423CFC3BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22050" windowHeight="8100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="22290" windowHeight="12000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1082,25 +1082,24 @@
     <t>Age at time of death [years]</t>
   </si>
   <si>
-    <t xml:space="preserve">If either parent has diabetes, the family history is marked as 1.
-If both parents do not have diabetes, the family history is marked as 0.                                                                                                                       If one parent's status is no or unknown (NA or 3), the family history is marked as 2. 
-If one parent's status is missing or unknown (NA or 3), the family history is marked as 2. </t>
+    <t>Sodium intake [mg/d]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sodium to potassium intake ratio </t>
   </si>
   <si>
     <t>case_when (
-  diabmut_15 == 1 | diabvat_15 == 1 ~ 1L,
-  diabmut_15 == 0 &amp; diabvat_15 == 0 ~ 0L,
-   diabmut_15 == 3 &amp; diabvat_15 == 0 ~ 2L,
-  diabvat_15 == 3 &amp; diabmut_15 == 0 ~ 2L,
-  (is.na(diabmut_15)  &amp;  diabvat_15 == 3 ~ 2L,                                                                          (is.na(diabvat_15)  &amp;  diabmut_15 == 3 ~ 2L, 
-  TRUE ~ NA_integer_
+      diabmut_15 == 1 | diabvat_15 == 1 ~ 1L,
+      diabmut_15 == 3 | diabvat_15 == 3 ~ 2L,
+      diabmut_15 == 2 &amp; diabvat_15 == 2 ~ 0L,
+      TRUE ~ NA_integer_
 )</t>
   </si>
   <si>
-    <t>Sodium intake [mg/d]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sodium to potassium intake ratio </t>
+    <t>If either parent has diabetes(1), the family history is marked as yes(1).
+If one parent's status is unknown (3), the family history is marked as don't know (2). 
+If both parents do not have diabetes (2), the family history is marked as no (0).
+Everything else (e.g. 2+ NA, NA+NA) is marked as NA</t>
   </si>
 </sst>
 </file>
@@ -1584,9 +1583,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C96" sqref="C96"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2500,7 +2499,7 @@
       </c>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:13" s="5" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2523,10 +2522,10 @@
         <v>27</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>29</v>
@@ -4539,7 +4538,7 @@
         <v>216</v>
       </c>
       <c r="C95" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D95" t="s">
         <v>22</v>
@@ -4572,7 +4571,7 @@
         <v>218</v>
       </c>
       <c r="C96" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D96" t="s">
         <v>22</v>
@@ -5095,27 +5094,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -5356,26 +5334,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF2265-5030-4B54-A34F-4798AFD4DA4C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{398CA3EE-638E-435F-8CA6-D67A7B863103}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2AE2FD3-517E-4530-8BC5-1FF35C67F615}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5392,4 +5372,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{398CA3EE-638E-435F-8CA6-D67A7B863103}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF2265-5030-4B54-A34F-4798AFD4DA4C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GL-4 DPE_GINI_P2 updated FAM_DIAB2 (need to update EDU_LEVEL)
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_GINI_P2.xlsx
+++ b/rmonize/data_proc_elem/DPE_GINI_P2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632AF36A-8C99-4887-8FCF-B7423CFC3BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E42FA2B-B7B4-4F06-B7B4-ED3554A8C177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="22290" windowHeight="12000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="22260" windowHeight="12000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1090,16 +1090,16 @@
   <si>
     <t>case_when (
       diabmut_15 == 1 | diabvat_15 == 1 ~ 1L,
+      diabmut_15 == 2 | diabvat_15 == 2 ~ 0L,
       diabmut_15 == 3 | diabvat_15 == 3 ~ 2L,
-      diabmut_15 == 2 &amp; diabvat_15 == 2 ~ 0L,
       TRUE ~ NA_integer_
 )</t>
   </si>
   <si>
-    <t>If either parent has diabetes(1), the family history is marked as yes(1).
-If one parent's status is unknown (3), the family history is marked as don't know (2). 
-If both parents do not have diabetes (2), the family history is marked as no (0).
-Everything else (e.g. 2+ NA, NA+NA) is marked as NA</t>
+    <t>If either parent has diabetes (coded as 1), the family history is marked as Yes (1).
+If both parents do not have diabetes (coded as 2), and condition 1 does not apply, the family history is marked as No (0).
+If either parent's diabetes status is unknown (coded as 3), and conditions 1 and 2 do not apply, the family history is marked as Don't Know (2).
+All other cases are marked as NA.</t>
   </si>
 </sst>
 </file>
@@ -1583,9 +1583,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H29" sqref="H29:I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5094,6 +5094,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -5334,28 +5355,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF2265-5030-4B54-A34F-4798AFD4DA4C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{398CA3EE-638E-435F-8CA6-D67A7B863103}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2AE2FD3-517E-4530-8BC5-1FF35C67F615}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5372,23 +5391,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{398CA3EE-638E-435F-8CA6-D67A7B863103}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF2265-5030-4B54-A34F-4798AFD4DA4C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GL-4 DPE_GINI_P1+DPE_GINI_P2 updated EDU_LEVEL
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_GINI_P2.xlsx
+++ b/rmonize/data_proc_elem/DPE_GINI_P2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E42FA2B-B7B4-4F06-B7B4-ED3554A8C177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C0FE36-616F-490D-8C17-6C549426E018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="22260" windowHeight="12000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="22290" windowHeight="12000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -111,14 +111,6 @@
     <t>case_when</t>
   </si>
   <si>
-    <t>If both gsc09m (mother) and gsc08v (father) are NA, assign 5L ("not specified").
-If one parent has "other degree" (5) and the other parent has a valid level, use the valid level.
-If both have "other degree" (5), assign 5L.
-If one parent is NA, use the other parent’s value and map it directly.
-Both Present: Use the maximum value between the two parents (pmax), then map it to the appropriate category.
-Default: Assign NA_integer_ for unexpected cases (should not occur).</t>
-  </si>
-  <si>
     <t>partial</t>
   </si>
   <si>
@@ -830,42 +822,6 @@
   </si>
   <si>
     <t>recode(1=1; 2= 0;  ELSE = NA)</t>
-  </si>
-  <si>
-    <t>case_when(
-      is.na(gsc09m) &amp; is.na(gsc08v) ~ 5L,
-      gsc09m == 5 &amp; !is.na(gsc08v) ~ case_when(
-        gsc08v == 6 ~ 0L,
-        gsc08v == 1 ~ 1L,
-        gsc08v == 2 ~ 2L,
-        gsc08v == 3 ~ 3L,
-        gsc08v &gt;= 4 ~ 4L
-      ),
-      gsc08v == 5 &amp; !is.na(gsc09m) ~ case_when(
-        gsc09m == 6 ~ 0L,
-        gsc09m == 1 ~ 1L,
-        gsc09m == 2 ~ 2L,
-        gsc09m == 3 ~ 3L,
-        gsc09m &gt;= 4 ~ 4L
-      ),
-      gsc09m == 5 &amp; gsc08v == 5 ~ 5L,
-      is.na(gsc09m) &amp; gsc08v == 6 ~ 0L,
-      is.na(gsc09m) &amp; gsc08v == 1 ~ 1L,
-      is.na(gsc09m) &amp; gsc08v == 2 ~ 2L,
-      is.na(gsc09m) &amp; gsc08v == 3 ~ 3L,
-      is.na(gsc09m) &amp; gsc08v &gt;= 4 ~ 4L,
-      is.na(gsc08v) &amp; gsc09m == 6 ~ 0L,
-      is.na(gsc08v) &amp; gsc09m == 1 ~ 1L,
-      is.na(gsc08v) &amp; gsc09m == 2 ~ 2L,
-      is.na(gsc08v) &amp; gsc09m == 3 ~ 3L,
-      is.na(gsc08v) &amp; gsc09m &gt;= 4 ~ 4L,
-      pmax(gsc09m, gsc08v, na.rm = TRUE) == 6 ~ 0L,
-      pmax(gsc09m, gsc08v, na.rm = TRUE) == 1 ~ 1L,
-      pmax(gsc09m, gsc08v, na.rm = TRUE) == 2 ~ 2L,
-      pmax(gsc09m, gsc08v, na.rm = TRUE) == 3 ~ 3L,
-      pmax(gsc09m, gsc08v, na.rm = TRUE) &gt;= 4 ~ 4L,
-      TRUE ~ NA_integer_
-    )</t>
   </si>
   <si>
     <t>case_when (
@@ -1100,6 +1056,47 @@
 If both parents do not have diabetes (coded as 2), and condition 1 does not apply, the family history is marked as No (0).
 If either parent's diabetes status is unknown (coded as 3), and conditions 1 and 2 do not apply, the family history is marked as Don't Know (2).
 All other cases are marked as NA.</t>
+  </si>
+  <si>
+    <t>case_when(
+  is.na(gsc09m) &amp; is.na(gsc08v) ~ NA_integer_,
+  gsc09m == 5 &amp; gsc08v == 5 ~ 5L,
+  gsc09m == 5 &amp; !is.na(gsc08v) ~ case_when(
+    gsc08v == 6 ~ 0L,
+    gsc08v %in% 1:3 ~ 3L,
+    gsc08v == 4 ~ 4L,
+    TRUE ~ 5L
+  ),
+  gsc08v == 5 &amp; !is.na(gsc09m) ~ case_when(
+    gsc09m == 6 ~ 0L,
+    gsc09m %in% 1:3 ~ 3L,
+    gsc09m == 4 ~ 4L,
+    TRUE ~ 5L
+  ),
+  gsc09m == 5 &amp; gsc08v != 5  ~ case_when(
+    gsc08v == 6 ~ 0L,
+    gsc08v %in% 1:3 ~ 3L,
+    gsc08v == 4 ~ 4L,
+    TRUE ~ 5L
+  ),
+  gsc08v == 5 &amp; gsc09m != 5  ~ case_when(
+    gsc09m == 6 ~ 0L,
+    gsc09m %in% 1:3 ~ 3L,
+    gsc09m == 4 ~ 4L,
+    TRUE ~ 5L
+  ),
+  gsc09m == 6 | gsc08v == 6  ~ 0L,
+  gsc09m %in% 1:3 | gsc08v %in% 1:3 ~ 3L,
+  gsc09m == 4 | gsc08v == 4 ~ 4L,
+  TRUE ~ 5L
+)</t>
+  </si>
+  <si>
+    <t>Missing values: If both gsc09m and gsc08v are missing, it returns NA.
+Both are "not specified": If both are 5, it returns 5.
+One is "not specified": If one of the variables is 5 (i.e., "Sonstiger Abschluss"), it uses the other parent’s value (if valid) to determine the education level.
+One is missing: If one of the parents has a missing value (NA), it checks the valid level of the other parent.
+Max of both: If neither is missing, it will return the highest level between both parents (0L for none, 3L for secondary school, 4L for longer education).</t>
   </si>
 </sst>
 </file>
@@ -1162,17 +1159,20 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1217,7 +1217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1267,6 +1267,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1584,8 +1587,8 @@
   <dimension ref="A1:M131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H29" sqref="H29:I29"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1603,7 +1606,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -1710,7 +1713,7 @@
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D4" t="s">
         <v>22</v>
@@ -1732,7 +1735,7 @@
         <v>15</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -1757,17 +1760,17 @@
       <c r="G5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="15" t="s">
-        <v>258</v>
-      </c>
-      <c r="I5" s="2" t="s">
+      <c r="H5" s="25" t="s">
+        <v>326</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>327</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
@@ -1775,10 +1778,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
         <v>31</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -1787,22 +1790,22 @@
         <v>13</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>27</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="L6" s="2"/>
     </row>
@@ -1811,10 +1814,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
         <v>35</v>
-      </c>
-      <c r="C7" t="s">
-        <v>36</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -1823,22 +1826,22 @@
         <v>13</v>
       </c>
       <c r="F7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
         <v>37</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="I7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="14" t="s">
-        <v>40</v>
-      </c>
       <c r="J7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" t="s">
         <v>29</v>
-      </c>
-      <c r="K7" t="s">
-        <v>30</v>
       </c>
       <c r="L7" s="6"/>
     </row>
@@ -1847,10 +1850,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
@@ -1859,19 +1862,19 @@
         <v>13</v>
       </c>
       <c r="F8" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="H8" s="20" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1879,10 +1882,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
@@ -1891,17 +1894,17 @@
         <v>13</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I9" s="13"/>
       <c r="J9" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1909,10 +1912,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
         <v>48</v>
-      </c>
-      <c r="C10" t="s">
-        <v>49</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1921,19 +1924,19 @@
         <v>13</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1941,10 +1944,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
@@ -1953,16 +1956,16 @@
         <v>13</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1970,10 +1973,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D12" t="s">
         <v>22</v>
@@ -1982,16 +1985,16 @@
         <v>13</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1999,10 +2002,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D13" t="s">
         <v>22</v>
@@ -2011,16 +2014,16 @@
         <v>13</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2028,10 +2031,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
         <v>54</v>
-      </c>
-      <c r="C14" t="s">
-        <v>55</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
@@ -2040,22 +2043,22 @@
         <v>13</v>
       </c>
       <c r="F14" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>15</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2063,10 +2066,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" t="s">
         <v>58</v>
-      </c>
-      <c r="C15" t="s">
-        <v>59</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
@@ -2076,19 +2079,19 @@
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K15" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2096,10 +2099,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" t="s">
         <v>62</v>
-      </c>
-      <c r="C16" t="s">
-        <v>63</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
@@ -2108,16 +2111,16 @@
         <v>13</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2125,10 +2128,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
@@ -2138,16 +2141,16 @@
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2155,10 +2158,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
@@ -2167,16 +2170,16 @@
         <v>13</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -2184,10 +2187,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D19" t="s">
         <v>22</v>
@@ -2196,16 +2199,16 @@
         <v>13</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -2213,19 +2216,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" t="s">
+        <v>277</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>67</v>
-      </c>
-      <c r="C20" t="s">
-        <v>279</v>
-      </c>
-      <c r="D20" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>68</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>20</v>
@@ -2234,13 +2237,13 @@
         <v>20</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -2248,19 +2251,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" t="s">
+        <v>278</v>
+      </c>
+      <c r="D21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="C21" t="s">
-        <v>280</v>
-      </c>
-      <c r="D21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>71</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>20</v>
@@ -2269,13 +2272,13 @@
         <v>20</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K21" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -2283,19 +2286,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" t="s">
+        <v>279</v>
+      </c>
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="C22" t="s">
-        <v>281</v>
-      </c>
-      <c r="D22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>73</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>20</v>
@@ -2304,13 +2307,13 @@
         <v>20</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K22" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -2318,19 +2321,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" t="s">
+        <v>280</v>
+      </c>
+      <c r="D23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="C23" t="s">
-        <v>282</v>
-      </c>
-      <c r="D23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>75</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>20</v>
@@ -2339,13 +2342,13 @@
         <v>20</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K23" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -2353,10 +2356,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" t="s">
         <v>76</v>
-      </c>
-      <c r="C24" t="s">
-        <v>77</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
@@ -2365,16 +2368,16 @@
         <v>13</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -2382,10 +2385,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" t="s">
         <v>78</v>
-      </c>
-      <c r="C25" t="s">
-        <v>79</v>
       </c>
       <c r="D25" t="s">
         <v>12</v>
@@ -2394,16 +2397,16 @@
         <v>13</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -2411,10 +2414,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" t="s">
         <v>80</v>
-      </c>
-      <c r="C26" t="s">
-        <v>81</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
@@ -2423,16 +2426,16 @@
         <v>13</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2440,10 +2443,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" t="s">
         <v>82</v>
-      </c>
-      <c r="C27" t="s">
-        <v>83</v>
       </c>
       <c r="D27" t="s">
         <v>12</v>
@@ -2452,19 +2455,19 @@
         <v>13</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>15</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2472,10 +2475,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" t="s">
         <v>85</v>
-      </c>
-      <c r="C28" t="s">
-        <v>86</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
@@ -2485,17 +2488,17 @@
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I28" s="8"/>
       <c r="J28" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M28" s="2"/>
     </row>
@@ -2504,10 +2507,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" t="s">
         <v>87</v>
-      </c>
-      <c r="C29" t="s">
-        <v>88</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
@@ -2516,22 +2519,22 @@
         <v>13</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G29" s="19" t="s">
         <v>27</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K29" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="M29" s="6"/>
     </row>
@@ -2540,10 +2543,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" t="s">
         <v>90</v>
-      </c>
-      <c r="C30" t="s">
-        <v>91</v>
       </c>
       <c r="D30" t="s">
         <v>12</v>
@@ -2553,16 +2556,16 @@
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -2570,10 +2573,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" t="s">
         <v>92</v>
-      </c>
-      <c r="C31" t="s">
-        <v>93</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
@@ -2582,16 +2585,16 @@
         <v>13</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -2599,10 +2602,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" t="s">
         <v>94</v>
-      </c>
-      <c r="C32" t="s">
-        <v>95</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
@@ -2611,16 +2614,16 @@
         <v>13</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -2628,10 +2631,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" t="s">
         <v>96</v>
-      </c>
-      <c r="C33" t="s">
-        <v>97</v>
       </c>
       <c r="D33" t="s">
         <v>12</v>
@@ -2640,16 +2643,16 @@
         <v>13</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -2657,10 +2660,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" t="s">
         <v>98</v>
-      </c>
-      <c r="C34" t="s">
-        <v>99</v>
       </c>
       <c r="D34" t="s">
         <v>12</v>
@@ -2669,16 +2672,16 @@
         <v>13</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -2686,10 +2689,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C35" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D35" t="s">
         <v>12</v>
@@ -2698,16 +2701,16 @@
         <v>13</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2715,10 +2718,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C36" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D36" t="s">
         <v>12</v>
@@ -2727,16 +2730,16 @@
         <v>13</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2744,10 +2747,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C37" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D37" t="s">
         <v>12</v>
@@ -2756,16 +2759,16 @@
         <v>13</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -2773,10 +2776,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38" t="s">
         <v>103</v>
-      </c>
-      <c r="C38" t="s">
-        <v>104</v>
       </c>
       <c r="D38" t="s">
         <v>12</v>
@@ -2785,16 +2788,16 @@
         <v>13</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -2802,10 +2805,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" t="s">
         <v>105</v>
-      </c>
-      <c r="C39" t="s">
-        <v>106</v>
       </c>
       <c r="D39" t="s">
         <v>12</v>
@@ -2814,16 +2817,16 @@
         <v>13</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2831,10 +2834,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C40" t="s">
         <v>107</v>
-      </c>
-      <c r="C40" t="s">
-        <v>108</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
@@ -2843,16 +2846,16 @@
         <v>13</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -2860,10 +2863,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C41" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D41" t="s">
         <v>22</v>
@@ -2872,16 +2875,16 @@
         <v>13</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -2889,10 +2892,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" t="s">
         <v>110</v>
-      </c>
-      <c r="C42" t="s">
-        <v>111</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
@@ -2901,16 +2904,16 @@
         <v>13</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -2918,10 +2921,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C43" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D43" t="s">
         <v>22</v>
@@ -2930,16 +2933,16 @@
         <v>13</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -2947,10 +2950,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>112</v>
+      </c>
+      <c r="C44" t="s">
         <v>113</v>
-      </c>
-      <c r="C44" t="s">
-        <v>114</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
@@ -2959,16 +2962,16 @@
         <v>13</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -2976,10 +2979,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C45" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D45" t="s">
         <v>22</v>
@@ -2988,16 +2991,16 @@
         <v>13</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -3005,10 +3008,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C46" t="s">
         <v>116</v>
-      </c>
-      <c r="C46" t="s">
-        <v>117</v>
       </c>
       <c r="D46" t="s">
         <v>12</v>
@@ -3017,16 +3020,16 @@
         <v>13</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -3034,10 +3037,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C47" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D47" t="s">
         <v>22</v>
@@ -3046,16 +3049,16 @@
         <v>13</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -3063,10 +3066,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C48" t="s">
         <v>119</v>
-      </c>
-      <c r="C48" t="s">
-        <v>120</v>
       </c>
       <c r="D48" t="s">
         <v>12</v>
@@ -3075,16 +3078,16 @@
         <v>13</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -3092,10 +3095,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C49" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D49" t="s">
         <v>22</v>
@@ -3104,16 +3107,16 @@
         <v>13</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -3121,10 +3124,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C50" t="s">
         <v>122</v>
-      </c>
-      <c r="C50" t="s">
-        <v>123</v>
       </c>
       <c r="D50" t="s">
         <v>12</v>
@@ -3133,16 +3136,16 @@
         <v>13</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -3150,10 +3153,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C51" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D51" t="s">
         <v>22</v>
@@ -3162,16 +3165,16 @@
         <v>13</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -3179,10 +3182,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C52" t="s">
         <v>125</v>
-      </c>
-      <c r="C52" t="s">
-        <v>126</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
@@ -3191,16 +3194,16 @@
         <v>13</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -3208,10 +3211,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C53" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D53" t="s">
         <v>22</v>
@@ -3220,16 +3223,16 @@
         <v>13</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -3237,10 +3240,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C54" t="s">
         <v>128</v>
-      </c>
-      <c r="C54" t="s">
-        <v>129</v>
       </c>
       <c r="D54" t="s">
         <v>12</v>
@@ -3249,16 +3252,16 @@
         <v>13</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -3266,10 +3269,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C55" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D55" t="s">
         <v>22</v>
@@ -3278,16 +3281,16 @@
         <v>13</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -3295,10 +3298,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
+        <v>130</v>
+      </c>
+      <c r="C56" t="s">
         <v>131</v>
-      </c>
-      <c r="C56" t="s">
-        <v>132</v>
       </c>
       <c r="D56" t="s">
         <v>12</v>
@@ -3307,16 +3310,16 @@
         <v>13</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -3324,10 +3327,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C57" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D57" t="s">
         <v>22</v>
@@ -3336,16 +3339,16 @@
         <v>13</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3353,10 +3356,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C58" t="s">
         <v>134</v>
-      </c>
-      <c r="C58" t="s">
-        <v>135</v>
       </c>
       <c r="D58" t="s">
         <v>12</v>
@@ -3366,16 +3369,16 @@
       </c>
       <c r="F58" s="13"/>
       <c r="G58" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3383,28 +3386,28 @@
         <v>58</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C59" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D59" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3412,19 +3415,19 @@
         <v>59</v>
       </c>
       <c r="B60" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C60" t="s">
+        <v>320</v>
+      </c>
+      <c r="D60" t="s">
+        <v>22</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F60" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="C60" t="s">
-        <v>322</v>
-      </c>
-      <c r="D60" t="s">
-        <v>22</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>138</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>20</v>
@@ -3444,10 +3447,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C61" t="s">
         <v>139</v>
-      </c>
-      <c r="C61" t="s">
-        <v>140</v>
       </c>
       <c r="D61" t="s">
         <v>12</v>
@@ -3456,16 +3459,16 @@
         <v>13</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -3473,10 +3476,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C62" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D62" t="s">
         <v>22</v>
@@ -3485,16 +3488,16 @@
         <v>13</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -3502,10 +3505,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C63" t="s">
         <v>142</v>
-      </c>
-      <c r="C63" t="s">
-        <v>143</v>
       </c>
       <c r="D63" t="s">
         <v>12</v>
@@ -3514,16 +3517,16 @@
         <v>13</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -3531,10 +3534,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C64" t="s">
         <v>144</v>
-      </c>
-      <c r="C64" t="s">
-        <v>145</v>
       </c>
       <c r="D64" t="s">
         <v>12</v>
@@ -3543,16 +3546,16 @@
         <v>13</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
@@ -3560,19 +3563,19 @@
         <v>64</v>
       </c>
       <c r="B65" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C65" t="s">
+        <v>285</v>
+      </c>
+      <c r="D65" t="s">
+        <v>22</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="7" t="s">
         <v>146</v>
-      </c>
-      <c r="C65" t="s">
-        <v>287</v>
-      </c>
-      <c r="D65" t="s">
-        <v>22</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F65" s="7" t="s">
-        <v>147</v>
       </c>
       <c r="G65" s="7" t="s">
         <v>20</v>
@@ -3592,10 +3595,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C66" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D66" t="s">
         <v>22</v>
@@ -3604,7 +3607,7 @@
         <v>13</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G66" s="7" t="s">
         <v>20</v>
@@ -3625,10 +3628,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C67" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D67" t="s">
         <v>22</v>
@@ -3637,7 +3640,7 @@
         <v>13</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G67" s="7" t="s">
         <v>20</v>
@@ -3658,10 +3661,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C68" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D68" t="s">
         <v>22</v>
@@ -3670,7 +3673,7 @@
         <v>13</v>
       </c>
       <c r="F68" s="15" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G68" s="7" t="s">
         <v>20</v>
@@ -3683,7 +3686,7 @@
         <v>15</v>
       </c>
       <c r="K68" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3691,10 +3694,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C69" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D69" t="s">
         <v>22</v>
@@ -3704,17 +3707,17 @@
       </c>
       <c r="F69" s="9"/>
       <c r="G69" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I69"/>
       <c r="J69" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -3722,10 +3725,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C70" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D70" t="s">
         <v>22</v>
@@ -3735,17 +3738,17 @@
       </c>
       <c r="F70" s="7"/>
       <c r="G70" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I70" s="7"/>
       <c r="J70" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K70" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
@@ -3753,10 +3756,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C71" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D71" t="s">
         <v>22</v>
@@ -3766,17 +3769,17 @@
       </c>
       <c r="F71" s="7"/>
       <c r="G71" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H71" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I71" s="7"/>
       <c r="J71" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K71" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
@@ -3784,10 +3787,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C72" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D72" t="s">
         <v>22</v>
@@ -3797,17 +3800,17 @@
       </c>
       <c r="F72" s="7"/>
       <c r="G72" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H72" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I72" s="7"/>
       <c r="J72" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K72" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
@@ -3815,10 +3818,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C73" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D73" t="s">
         <v>22</v>
@@ -3828,17 +3831,17 @@
       </c>
       <c r="F73" s="7"/>
       <c r="G73" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H73" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I73" s="7"/>
       <c r="J73" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K73" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
@@ -3846,10 +3849,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C74" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D74" t="s">
         <v>22</v>
@@ -3859,17 +3862,17 @@
       </c>
       <c r="F74" s="7"/>
       <c r="G74" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H74" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I74" s="7"/>
       <c r="J74" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K74" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -3877,10 +3880,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C75" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D75" t="s">
         <v>22</v>
@@ -3889,7 +3892,7 @@
         <v>13</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G75" s="7" t="s">
         <v>20</v>
@@ -3910,10 +3913,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C76" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D76" t="s">
         <v>22</v>
@@ -3923,17 +3926,17 @@
       </c>
       <c r="F76" s="7"/>
       <c r="G76" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H76" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I76" s="7"/>
       <c r="J76" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K76" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="77" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3941,19 +3944,19 @@
         <v>76</v>
       </c>
       <c r="B77" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C77" t="s">
+        <v>297</v>
+      </c>
+      <c r="D77" t="s">
+        <v>22</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F77" s="13" t="s">
         <v>159</v>
-      </c>
-      <c r="C77" t="s">
-        <v>299</v>
-      </c>
-      <c r="D77" t="s">
-        <v>22</v>
-      </c>
-      <c r="E77" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F77" s="13" t="s">
-        <v>160</v>
       </c>
       <c r="G77" s="7" t="s">
         <v>20</v>
@@ -3962,13 +3965,13 @@
         <v>20</v>
       </c>
       <c r="I77" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J77" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K77" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="78" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3976,10 +3979,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C78" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D78" t="s">
         <v>22</v>
@@ -3988,7 +3991,7 @@
         <v>13</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G78" s="7" t="s">
         <v>20</v>
@@ -4009,19 +4012,19 @@
         <v>78</v>
       </c>
       <c r="B79" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="C79" t="s">
         <v>163</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
+        <v>22</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F79" s="7" t="s">
         <v>164</v>
-      </c>
-      <c r="D79" t="s">
-        <v>22</v>
-      </c>
-      <c r="E79" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>165</v>
       </c>
       <c r="G79" s="7" t="s">
         <v>20</v>
@@ -4042,25 +4045,25 @@
         <v>79</v>
       </c>
       <c r="B80" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C80" t="s">
         <v>166</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D80" t="s">
+        <v>22</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F80" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="D80" t="s">
-        <v>22</v>
-      </c>
-      <c r="E80" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F80" s="7" t="s">
+      <c r="G80" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H80" s="7" t="s">
         <v>168</v>
-      </c>
-      <c r="G80" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H80" s="7" t="s">
-        <v>169</v>
       </c>
       <c r="I80" s="7"/>
       <c r="J80" s="7" t="s">
@@ -4075,25 +4078,25 @@
         <v>80</v>
       </c>
       <c r="B81" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C81" t="s">
         <v>170</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
+        <v>22</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F81" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="D81" t="s">
-        <v>22</v>
-      </c>
-      <c r="E81" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F81" s="7" t="s">
+      <c r="G81" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H81" s="7" t="s">
         <v>172</v>
-      </c>
-      <c r="G81" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H81" s="7" t="s">
-        <v>173</v>
       </c>
       <c r="I81" s="7"/>
       <c r="J81" s="7" t="s">
@@ -4108,25 +4111,25 @@
         <v>81</v>
       </c>
       <c r="B82" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C82" t="s">
         <v>174</v>
       </c>
-      <c r="C82" t="s">
+      <c r="D82" t="s">
+        <v>22</v>
+      </c>
+      <c r="E82" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F82" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="D82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E82" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F82" s="7" t="s">
+      <c r="G82" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H82" s="7" t="s">
         <v>176</v>
-      </c>
-      <c r="G82" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H82" s="7" t="s">
-        <v>177</v>
       </c>
       <c r="I82" s="7"/>
       <c r="J82" s="7" t="s">
@@ -4141,25 +4144,25 @@
         <v>82</v>
       </c>
       <c r="B83" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C83" t="s">
         <v>178</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
+        <v>22</v>
+      </c>
+      <c r="E83" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F83" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D83" t="s">
-        <v>22</v>
-      </c>
-      <c r="E83" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F83" s="7" t="s">
+      <c r="G83" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H83" s="7" t="s">
         <v>180</v>
-      </c>
-      <c r="G83" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H83" s="7" t="s">
-        <v>181</v>
       </c>
       <c r="I83" s="7"/>
       <c r="J83" s="7" t="s">
@@ -4174,25 +4177,25 @@
         <v>83</v>
       </c>
       <c r="B84" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C84" t="s">
         <v>182</v>
       </c>
-      <c r="C84" t="s">
+      <c r="D84" t="s">
+        <v>22</v>
+      </c>
+      <c r="E84" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F84" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="D84" t="s">
-        <v>22</v>
-      </c>
-      <c r="E84" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F84" s="7" t="s">
+      <c r="G84" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H84" s="7" t="s">
         <v>184</v>
-      </c>
-      <c r="G84" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H84" s="7" t="s">
-        <v>185</v>
       </c>
       <c r="I84" s="7"/>
       <c r="J84" s="7" t="s">
@@ -4207,25 +4210,25 @@
         <v>84</v>
       </c>
       <c r="B85" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C85" t="s">
         <v>186</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D85" t="s">
+        <v>22</v>
+      </c>
+      <c r="E85" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F85" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="D85" t="s">
-        <v>22</v>
-      </c>
-      <c r="E85" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F85" s="7" t="s">
+      <c r="G85" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H85" s="7" t="s">
         <v>188</v>
-      </c>
-      <c r="G85" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H85" s="7" t="s">
-        <v>189</v>
       </c>
       <c r="I85" s="7"/>
       <c r="J85" s="7" t="s">
@@ -4240,25 +4243,25 @@
         <v>85</v>
       </c>
       <c r="B86" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C86" t="s">
         <v>190</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
+        <v>22</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F86" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="D86" t="s">
-        <v>22</v>
-      </c>
-      <c r="E86" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F86" s="7" t="s">
+      <c r="G86" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H86" s="7" t="s">
         <v>192</v>
-      </c>
-      <c r="G86" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H86" s="7" t="s">
-        <v>193</v>
       </c>
       <c r="I86" s="7"/>
       <c r="J86" s="7" t="s">
@@ -4273,25 +4276,25 @@
         <v>86</v>
       </c>
       <c r="B87" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C87" t="s">
         <v>194</v>
       </c>
-      <c r="C87" t="s">
+      <c r="D87" t="s">
+        <v>22</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F87" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D87" t="s">
-        <v>22</v>
-      </c>
-      <c r="E87" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F87" s="7" t="s">
+      <c r="G87" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H87" s="7" t="s">
         <v>196</v>
-      </c>
-      <c r="G87" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H87" s="7" t="s">
-        <v>197</v>
       </c>
       <c r="I87" s="7"/>
       <c r="J87" s="7" t="s">
@@ -4306,10 +4309,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C88" t="s">
         <v>198</v>
-      </c>
-      <c r="C88" t="s">
-        <v>199</v>
       </c>
       <c r="D88" t="s">
         <v>22</v>
@@ -4319,17 +4322,17 @@
       </c>
       <c r="F88" s="7"/>
       <c r="G88" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H88" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I88" s="7"/>
       <c r="J88" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K88" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
@@ -4337,10 +4340,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C89" t="s">
         <v>200</v>
-      </c>
-      <c r="C89" t="s">
-        <v>201</v>
       </c>
       <c r="D89" t="s">
         <v>22</v>
@@ -4350,17 +4353,17 @@
       </c>
       <c r="F89" s="7"/>
       <c r="G89" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H89" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I89" s="7"/>
       <c r="J89" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K89" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
@@ -4368,10 +4371,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C90" t="s">
         <v>202</v>
-      </c>
-      <c r="C90" t="s">
-        <v>203</v>
       </c>
       <c r="D90" t="s">
         <v>22</v>
@@ -4381,17 +4384,17 @@
       </c>
       <c r="F90" s="7"/>
       <c r="G90" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I90" s="7"/>
       <c r="J90" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K90" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
@@ -4399,25 +4402,25 @@
         <v>90</v>
       </c>
       <c r="B91" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C91" t="s">
         <v>204</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F91" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="D91" t="s">
-        <v>22</v>
-      </c>
-      <c r="E91" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F91" s="7" t="s">
+      <c r="G91" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H91" s="7" t="s">
         <v>206</v>
-      </c>
-      <c r="G91" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H91" s="7" t="s">
-        <v>207</v>
       </c>
       <c r="I91" s="7"/>
       <c r="J91" s="7" t="s">
@@ -4432,25 +4435,25 @@
         <v>91</v>
       </c>
       <c r="B92" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C92" t="s">
         <v>208</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D92" t="s">
+        <v>22</v>
+      </c>
+      <c r="E92" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F92" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="D92" t="s">
-        <v>22</v>
-      </c>
-      <c r="E92" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F92" s="7" t="s">
+      <c r="G92" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H92" s="7" t="s">
         <v>210</v>
-      </c>
-      <c r="G92" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H92" s="7" t="s">
-        <v>211</v>
       </c>
       <c r="I92" s="7"/>
       <c r="J92" s="7" t="s">
@@ -4465,11 +4468,11 @@
         <v>92</v>
       </c>
       <c r="B93" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C93" t="s">
         <v>212</v>
       </c>
-      <c r="C93" t="s">
-        <v>213</v>
-      </c>
       <c r="D93" t="s">
         <v>22</v>
       </c>
@@ -4477,7 +4480,7 @@
         <v>13</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>20</v>
@@ -4486,7 +4489,7 @@
         <v>20</v>
       </c>
       <c r="I93" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J93" s="7" t="s">
         <v>15</v>
@@ -4500,10 +4503,10 @@
         <v>93</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C94" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D94" t="s">
         <v>22</v>
@@ -4512,7 +4515,7 @@
         <v>13</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>20</v>
@@ -4521,7 +4524,7 @@
         <v>20</v>
       </c>
       <c r="I94" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J94" s="7" t="s">
         <v>15</v>
@@ -4535,19 +4538,19 @@
         <v>94</v>
       </c>
       <c r="B95" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C95" t="s">
+        <v>322</v>
+      </c>
+      <c r="D95" t="s">
+        <v>22</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F95" s="7" t="s">
         <v>216</v>
-      </c>
-      <c r="C95" t="s">
-        <v>324</v>
-      </c>
-      <c r="D95" t="s">
-        <v>22</v>
-      </c>
-      <c r="E95" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F95" s="7" t="s">
-        <v>217</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>20</v>
@@ -4568,25 +4571,25 @@
         <v>95</v>
       </c>
       <c r="B96" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="C96" t="s">
+        <v>323</v>
+      </c>
+      <c r="D96" t="s">
+        <v>22</v>
+      </c>
+      <c r="E96" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F96" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="C96" t="s">
-        <v>325</v>
-      </c>
-      <c r="D96" t="s">
-        <v>22</v>
-      </c>
-      <c r="E96" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F96" s="7" t="s">
+      <c r="G96" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H96" s="7" t="s">
         <v>219</v>
-      </c>
-      <c r="G96" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H96" s="7" t="s">
-        <v>220</v>
       </c>
       <c r="I96" s="7"/>
       <c r="J96" s="7" t="s">
@@ -4601,32 +4604,32 @@
         <v>96</v>
       </c>
       <c r="B97" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C97" t="s">
         <v>221</v>
       </c>
-      <c r="C97" t="s">
+      <c r="D97" t="s">
+        <v>22</v>
+      </c>
+      <c r="E97" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F97" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="G97" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H97" s="15" t="s">
         <v>222</v>
-      </c>
-      <c r="D97" t="s">
-        <v>22</v>
-      </c>
-      <c r="E97" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F97" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="G97" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H97" s="15" t="s">
-        <v>223</v>
       </c>
       <c r="I97" s="7"/>
       <c r="J97" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K97" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="98" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -4634,10 +4637,10 @@
         <v>97</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C98" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D98" t="s">
         <v>22</v>
@@ -4646,20 +4649,20 @@
         <v>13</v>
       </c>
       <c r="F98" s="15" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G98" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H98" s="15" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="I98" s="7"/>
       <c r="J98" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K98" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
@@ -4667,32 +4670,32 @@
         <v>98</v>
       </c>
       <c r="B99" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="C99" t="s">
+        <v>301</v>
+      </c>
+      <c r="D99" t="s">
+        <v>22</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F99" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="C99" t="s">
-        <v>303</v>
-      </c>
-      <c r="D99" t="s">
-        <v>22</v>
-      </c>
-      <c r="E99" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F99" s="7" t="s">
+      <c r="G99" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H99" s="7" t="s">
         <v>226</v>
-      </c>
-      <c r="G99" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H99" s="7" t="s">
-        <v>227</v>
       </c>
       <c r="I99" s="7"/>
       <c r="J99" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K99" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
@@ -4700,32 +4703,32 @@
         <v>99</v>
       </c>
       <c r="B100" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C100" t="s">
+        <v>302</v>
+      </c>
+      <c r="D100" t="s">
+        <v>22</v>
+      </c>
+      <c r="E100" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F100" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="C100" t="s">
-        <v>304</v>
-      </c>
-      <c r="D100" t="s">
-        <v>22</v>
-      </c>
-      <c r="E100" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F100" s="7" t="s">
+      <c r="G100" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H100" s="7" t="s">
         <v>229</v>
-      </c>
-      <c r="G100" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H100" s="7" t="s">
-        <v>230</v>
       </c>
       <c r="I100" s="7"/>
       <c r="J100" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K100" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
@@ -4733,10 +4736,10 @@
         <v>100</v>
       </c>
       <c r="B101" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="C101" t="s">
         <v>231</v>
-      </c>
-      <c r="C101" t="s">
-        <v>232</v>
       </c>
       <c r="D101" t="s">
         <v>22</v>
@@ -4746,17 +4749,17 @@
       </c>
       <c r="F101" s="7"/>
       <c r="G101" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I101" s="7"/>
       <c r="J101" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K101" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
@@ -4764,32 +4767,32 @@
         <v>101</v>
       </c>
       <c r="B102" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="C102" t="s">
         <v>233</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D102" t="s">
+        <v>22</v>
+      </c>
+      <c r="E102" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F102" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="D102" t="s">
-        <v>22</v>
-      </c>
-      <c r="E102" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F102" s="7" t="s">
+      <c r="G102" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H102" s="7" t="s">
         <v>235</v>
-      </c>
-      <c r="G102" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H102" s="7" t="s">
-        <v>236</v>
       </c>
       <c r="I102" s="7"/>
       <c r="J102" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K102" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
@@ -4797,10 +4800,10 @@
         <v>102</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C103" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D103" t="s">
         <v>22</v>
@@ -4810,17 +4813,17 @@
       </c>
       <c r="F103" s="7"/>
       <c r="G103" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H103" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I103" s="7"/>
       <c r="J103" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K103" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="104" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -4828,10 +4831,10 @@
         <v>103</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C104" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D104" t="s">
         <v>22</v>
@@ -4840,20 +4843,20 @@
         <v>13</v>
       </c>
       <c r="F104" s="7" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G104" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H104" s="15" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I104" s="7"/>
       <c r="J104" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K104" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
@@ -4861,11 +4864,11 @@
         <v>104</v>
       </c>
       <c r="B105" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C105" t="s">
         <v>239</v>
       </c>
-      <c r="C105" t="s">
-        <v>240</v>
-      </c>
       <c r="D105" t="s">
         <v>22</v>
       </c>
@@ -4873,20 +4876,20 @@
         <v>13</v>
       </c>
       <c r="F105" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G105" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H105" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I105" s="7"/>
       <c r="J105" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K105" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
@@ -4894,32 +4897,32 @@
         <v>105</v>
       </c>
       <c r="B106" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="C106" t="s">
         <v>241</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D106" t="s">
+        <v>22</v>
+      </c>
+      <c r="E106" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F106" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="D106" t="s">
-        <v>22</v>
-      </c>
-      <c r="E106" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F106" s="7" t="s">
+      <c r="G106" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H106" s="7" t="s">
         <v>243</v>
-      </c>
-      <c r="G106" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H106" s="7" t="s">
-        <v>244</v>
       </c>
       <c r="I106" s="7"/>
       <c r="J106" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K106" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
@@ -4927,10 +4930,10 @@
         <v>106</v>
       </c>
       <c r="B107" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C107" t="s">
         <v>245</v>
-      </c>
-      <c r="C107" t="s">
-        <v>246</v>
       </c>
       <c r="D107" t="s">
         <v>22</v>
@@ -4940,17 +4943,17 @@
       </c>
       <c r="F107" s="7"/>
       <c r="G107" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H107" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I107" s="7"/>
       <c r="J107" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K107" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
@@ -4958,19 +4961,19 @@
         <v>107</v>
       </c>
       <c r="B108" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C108" t="s">
         <v>247</v>
       </c>
-      <c r="C108" t="s">
+      <c r="D108" t="s">
+        <v>22</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F108" s="7" t="s">
         <v>248</v>
-      </c>
-      <c r="D108" t="s">
-        <v>22</v>
-      </c>
-      <c r="E108" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F108" s="7" t="s">
-        <v>249</v>
       </c>
       <c r="G108" s="7" t="s">
         <v>20</v>
@@ -4991,10 +4994,10 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
+        <v>249</v>
+      </c>
+      <c r="C109" t="s">
         <v>250</v>
-      </c>
-      <c r="C109" t="s">
-        <v>251</v>
       </c>
       <c r="D109" t="s">
         <v>12</v>
@@ -5003,16 +5006,16 @@
         <v>13</v>
       </c>
       <c r="F109" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="G109" s="3" t="s">
         <v>252</v>
-      </c>
-      <c r="G109" s="3" t="s">
-        <v>253</v>
       </c>
       <c r="H109">
         <v>1</v>
       </c>
       <c r="I109" s="24" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J109" s="12" t="s">
         <v>15</v>
@@ -5094,27 +5097,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -5355,26 +5337,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF2265-5030-4B54-A34F-4798AFD4DA4C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{398CA3EE-638E-435F-8CA6-D67A7B863103}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2AE2FD3-517E-4530-8BC5-1FF35C67F615}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5391,4 +5375,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{398CA3EE-638E-435F-8CA6-D67A7B863103}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF2265-5030-4B54-A34F-4798AFD4DA4C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GL-5 change in DPE + new mock data sets
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_GINI_P2.xlsx
+++ b/rmonize/data_proc_elem/DPE_GINI_P2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_proc_elem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C0FE36-616F-490D-8C17-6C549426E018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CC080C-5B3C-4740-A94E-9B52542DE142}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="22290" windowHeight="12000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,9 +105,6 @@
     <t>Education</t>
   </si>
   <si>
-    <t>gsc09m; gsc08v</t>
-  </si>
-  <si>
     <t>case_when</t>
   </si>
   <si>
@@ -1059,44 +1056,23 @@
   </si>
   <si>
     <t>case_when(
-  is.na(gsc09m) &amp; is.na(gsc08v) ~ NA_integer_,
-  gsc09m == 5 &amp; gsc08v == 5 ~ 5L,
-  gsc09m == 5 &amp; !is.na(gsc08v) ~ case_when(
-    gsc08v == 6 ~ 0L,
-    gsc08v %in% 1:3 ~ 3L,
-    gsc08v == 4 ~ 4L,
-    TRUE ~ 5L
-  ),
-  gsc08v == 5 &amp; !is.na(gsc09m) ~ case_when(
-    gsc09m == 6 ~ 0L,
-    gsc09m %in% 1:3 ~ 3L,
-    gsc09m == 4 ~ 4L,
-    TRUE ~ 5L
-  ),
-  gsc09m == 5 &amp; gsc08v != 5  ~ case_when(
-    gsc08v == 6 ~ 0L,
-    gsc08v %in% 1:3 ~ 3L,
-    gsc08v == 4 ~ 4L,
-    TRUE ~ 5L
-  ),
-  gsc08v == 5 &amp; gsc09m != 5  ~ case_when(
-    gsc09m == 6 ~ 0L,
-    gsc09m %in% 1:3 ~ 3L,
-    gsc09m == 4 ~ 4L,
-    TRUE ~ 5L
-  ),
-  gsc09m == 6 | gsc08v == 6  ~ 0L,
-  gsc09m %in% 1:3 | gsc08v %in% 1:3 ~ 3L,
-  gsc09m == 4 | gsc08v == 4 ~ 4L,
-  TRUE ~ 5L
-)</t>
-  </si>
-  <si>
-    <t>Missing values: If both gsc09m and gsc08v are missing, it returns NA.
-Both are "not specified": If both are 5, it returns 5.
-One is "not specified": If one of the variables is 5 (i.e., "Sonstiger Abschluss"), it uses the other parent’s value (if valid) to determine the education level.
-One is missing: If one of the parents has a missing value (NA), it checks the valid level of the other parent.
-Max of both: If neither is missing, it will return the highest level between both parents (0L for none, 3L for secondary school, 4L for longer education).</t>
+  MUTBERU_3 %in% c(7) | VATBERU_3 %in% c(7) ~ 7L,
+  MUTBERU_3 %in% c(5,6) | VATBERU_3 %in% c(5,6) ~ 6L,
+  MUTBERU_3 %in% c(3,4) |VATBERU_3 %in% c(3,4) ~ 4L,
+  MUTBERU_3 %in% c(8) |VATBERU_3 %in% c(8) ~ 9L,
+  gsc09m %in% c(3) | gsc08v %in% c(3) ~ 3L,
+  gsc09m %in% c(1,2) | gsc08v %in% c(1,2) ~ 2L,
+  gsc09m %in% c(6) &amp; gsc08v %in% c(6) ~ 0L,
+  is.na(gsc09m) &amp; gsc08v %in% c(6) ~ 0L,
+  gsc09m %in% c(6) &amp; is.na(gsc08v) ~ 0L,
+  gsc09m %in% c(5) | gsc08v %in% c(5) ~ 9L,
+  TRUE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>gsc09m; gsc08v; MUTBERU_3; VATBERU_3</t>
+  </si>
+  <si>
+    <t>Education according to the ISCED 2011 classification</t>
   </si>
 </sst>
 </file>
@@ -1272,7 +1248,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1586,12 +1562,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5:K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="81.5703125" bestFit="1" customWidth="1"/>
@@ -1606,7 +1582,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -1713,7 +1689,7 @@
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D4" t="s">
         <v>22</v>
@@ -1735,10 +1711,10 @@
         <v>15</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1755,22 +1731,22 @@
         <v>13</v>
       </c>
       <c r="F5" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>27</v>
-      </c>
       <c r="H5" s="25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I5" s="16" t="s">
         <v>327</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
@@ -1778,10 +1754,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
         <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -1790,22 +1766,22 @@
         <v>13</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="I6" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="15" t="s">
-        <v>257</v>
-      </c>
-      <c r="I6" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="L6" s="2"/>
     </row>
@@ -1814,10 +1790,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
         <v>34</v>
-      </c>
-      <c r="C7" t="s">
-        <v>35</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -1826,22 +1802,22 @@
         <v>13</v>
       </c>
       <c r="F7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" t="s">
         <v>36</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="I7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="14" t="s">
-        <v>39</v>
-      </c>
       <c r="J7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" t="s">
         <v>28</v>
-      </c>
-      <c r="K7" t="s">
-        <v>29</v>
       </c>
       <c r="L7" s="6"/>
     </row>
@@ -1850,10 +1826,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
@@ -1862,19 +1838,19 @@
         <v>13</v>
       </c>
       <c r="F8" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="H8" s="20" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1882,10 +1858,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
@@ -1894,17 +1870,17 @@
         <v>13</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I9" s="13"/>
       <c r="J9" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1912,10 +1888,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
         <v>47</v>
-      </c>
-      <c r="C10" t="s">
-        <v>48</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -1924,19 +1900,19 @@
         <v>13</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1944,10 +1920,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
@@ -1956,16 +1932,16 @@
         <v>13</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1973,10 +1949,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D12" t="s">
         <v>22</v>
@@ -1985,16 +1961,16 @@
         <v>13</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2002,10 +1978,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D13" t="s">
         <v>22</v>
@@ -2014,16 +1990,16 @@
         <v>13</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2031,10 +2007,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
         <v>53</v>
-      </c>
-      <c r="C14" t="s">
-        <v>54</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
@@ -2043,22 +2019,22 @@
         <v>13</v>
       </c>
       <c r="F14" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>15</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2066,10 +2042,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
         <v>57</v>
-      </c>
-      <c r="C15" t="s">
-        <v>58</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
@@ -2079,19 +2055,19 @@
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2099,10 +2075,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" t="s">
         <v>61</v>
-      </c>
-      <c r="C16" t="s">
-        <v>62</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
@@ -2111,16 +2087,16 @@
         <v>13</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2128,10 +2104,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
@@ -2141,16 +2117,16 @@
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2158,10 +2134,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
@@ -2170,16 +2146,16 @@
         <v>13</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -2187,10 +2163,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D19" t="s">
         <v>22</v>
@@ -2199,16 +2175,16 @@
         <v>13</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -2216,19 +2192,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" t="s">
+        <v>276</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="C20" t="s">
-        <v>277</v>
-      </c>
-      <c r="D20" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>67</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>20</v>
@@ -2237,13 +2213,13 @@
         <v>20</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -2251,19 +2227,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" t="s">
+        <v>277</v>
+      </c>
+      <c r="D21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="C21" t="s">
-        <v>278</v>
-      </c>
-      <c r="D21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>20</v>
@@ -2272,13 +2248,13 @@
         <v>20</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J21" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K21" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -2286,19 +2262,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" t="s">
+        <v>278</v>
+      </c>
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="C22" t="s">
-        <v>279</v>
-      </c>
-      <c r="D22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>20</v>
@@ -2307,13 +2283,13 @@
         <v>20</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -2321,19 +2297,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" t="s">
+        <v>279</v>
+      </c>
+      <c r="D23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="C23" t="s">
-        <v>280</v>
-      </c>
-      <c r="D23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>20</v>
@@ -2342,13 +2318,13 @@
         <v>20</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J23" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K23" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -2356,10 +2332,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" t="s">
         <v>75</v>
-      </c>
-      <c r="C24" t="s">
-        <v>76</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
@@ -2368,16 +2344,16 @@
         <v>13</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -2385,10 +2361,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" t="s">
         <v>77</v>
-      </c>
-      <c r="C25" t="s">
-        <v>78</v>
       </c>
       <c r="D25" t="s">
         <v>12</v>
@@ -2397,16 +2373,16 @@
         <v>13</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -2414,10 +2390,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" t="s">
         <v>79</v>
-      </c>
-      <c r="C26" t="s">
-        <v>80</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
@@ -2426,16 +2402,16 @@
         <v>13</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2443,10 +2419,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" t="s">
         <v>81</v>
-      </c>
-      <c r="C27" t="s">
-        <v>82</v>
       </c>
       <c r="D27" t="s">
         <v>12</v>
@@ -2455,19 +2431,19 @@
         <v>13</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>15</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2475,10 +2451,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" t="s">
         <v>84</v>
-      </c>
-      <c r="C28" t="s">
-        <v>85</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
@@ -2488,17 +2464,17 @@
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I28" s="8"/>
       <c r="J28" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M28" s="2"/>
     </row>
@@ -2507,10 +2483,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" t="s">
         <v>86</v>
-      </c>
-      <c r="C29" t="s">
-        <v>87</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
@@ -2519,22 +2495,22 @@
         <v>13</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G29" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>323</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="J29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H29" s="17" t="s">
-        <v>324</v>
-      </c>
-      <c r="I29" s="18" t="s">
-        <v>325</v>
-      </c>
-      <c r="J29" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="M29" s="6"/>
     </row>
@@ -2543,10 +2519,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" t="s">
         <v>89</v>
-      </c>
-      <c r="C30" t="s">
-        <v>90</v>
       </c>
       <c r="D30" t="s">
         <v>12</v>
@@ -2556,16 +2532,16 @@
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -2573,10 +2549,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" t="s">
         <v>91</v>
-      </c>
-      <c r="C31" t="s">
-        <v>92</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
@@ -2585,16 +2561,16 @@
         <v>13</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -2602,10 +2578,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" t="s">
         <v>93</v>
-      </c>
-      <c r="C32" t="s">
-        <v>94</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
@@ -2614,16 +2590,16 @@
         <v>13</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -2631,10 +2607,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" t="s">
         <v>95</v>
-      </c>
-      <c r="C33" t="s">
-        <v>96</v>
       </c>
       <c r="D33" t="s">
         <v>12</v>
@@ -2643,16 +2619,16 @@
         <v>13</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -2660,10 +2636,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" t="s">
         <v>97</v>
-      </c>
-      <c r="C34" t="s">
-        <v>98</v>
       </c>
       <c r="D34" t="s">
         <v>12</v>
@@ -2672,16 +2648,16 @@
         <v>13</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -2689,10 +2665,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C35" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D35" t="s">
         <v>12</v>
@@ -2701,16 +2677,16 @@
         <v>13</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -2718,10 +2694,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C36" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D36" t="s">
         <v>12</v>
@@ -2730,16 +2706,16 @@
         <v>13</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2747,10 +2723,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C37" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D37" t="s">
         <v>12</v>
@@ -2759,16 +2735,16 @@
         <v>13</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -2776,10 +2752,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" t="s">
         <v>102</v>
-      </c>
-      <c r="C38" t="s">
-        <v>103</v>
       </c>
       <c r="D38" t="s">
         <v>12</v>
@@ -2788,16 +2764,16 @@
         <v>13</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -2805,10 +2781,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" t="s">
         <v>104</v>
-      </c>
-      <c r="C39" t="s">
-        <v>105</v>
       </c>
       <c r="D39" t="s">
         <v>12</v>
@@ -2817,16 +2793,16 @@
         <v>13</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -2834,10 +2810,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" t="s">
         <v>106</v>
-      </c>
-      <c r="C40" t="s">
-        <v>107</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
@@ -2846,16 +2822,16 @@
         <v>13</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -2863,10 +2839,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C41" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D41" t="s">
         <v>22</v>
@@ -2875,16 +2851,16 @@
         <v>13</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -2892,10 +2868,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" t="s">
         <v>109</v>
-      </c>
-      <c r="C42" t="s">
-        <v>110</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
@@ -2904,16 +2880,16 @@
         <v>13</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -2921,10 +2897,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C43" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D43" t="s">
         <v>22</v>
@@ -2933,16 +2909,16 @@
         <v>13</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -2950,10 +2926,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44" t="s">
         <v>112</v>
-      </c>
-      <c r="C44" t="s">
-        <v>113</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
@@ -2962,16 +2938,16 @@
         <v>13</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -2979,10 +2955,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C45" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D45" t="s">
         <v>22</v>
@@ -2991,16 +2967,16 @@
         <v>13</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -3008,10 +2984,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C46" t="s">
         <v>115</v>
-      </c>
-      <c r="C46" t="s">
-        <v>116</v>
       </c>
       <c r="D46" t="s">
         <v>12</v>
@@ -3020,16 +2996,16 @@
         <v>13</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -3037,10 +3013,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C47" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D47" t="s">
         <v>22</v>
@@ -3049,16 +3025,16 @@
         <v>13</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -3066,10 +3042,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C48" t="s">
         <v>118</v>
-      </c>
-      <c r="C48" t="s">
-        <v>119</v>
       </c>
       <c r="D48" t="s">
         <v>12</v>
@@ -3078,16 +3054,16 @@
         <v>13</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -3095,10 +3071,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C49" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D49" t="s">
         <v>22</v>
@@ -3107,16 +3083,16 @@
         <v>13</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -3124,10 +3100,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C50" t="s">
         <v>121</v>
-      </c>
-      <c r="C50" t="s">
-        <v>122</v>
       </c>
       <c r="D50" t="s">
         <v>12</v>
@@ -3136,16 +3112,16 @@
         <v>13</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -3153,10 +3129,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C51" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D51" t="s">
         <v>22</v>
@@ -3165,16 +3141,16 @@
         <v>13</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -3182,10 +3158,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C52" t="s">
         <v>124</v>
-      </c>
-      <c r="C52" t="s">
-        <v>125</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
@@ -3194,16 +3170,16 @@
         <v>13</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -3211,10 +3187,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C53" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D53" t="s">
         <v>22</v>
@@ -3223,16 +3199,16 @@
         <v>13</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -3240,10 +3216,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C54" t="s">
         <v>127</v>
-      </c>
-      <c r="C54" t="s">
-        <v>128</v>
       </c>
       <c r="D54" t="s">
         <v>12</v>
@@ -3252,16 +3228,16 @@
         <v>13</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -3269,10 +3245,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C55" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D55" t="s">
         <v>22</v>
@@ -3281,16 +3257,16 @@
         <v>13</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -3298,10 +3274,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
+        <v>129</v>
+      </c>
+      <c r="C56" t="s">
         <v>130</v>
-      </c>
-      <c r="C56" t="s">
-        <v>131</v>
       </c>
       <c r="D56" t="s">
         <v>12</v>
@@ -3310,16 +3286,16 @@
         <v>13</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -3327,10 +3303,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C57" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D57" t="s">
         <v>22</v>
@@ -3339,16 +3315,16 @@
         <v>13</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3356,10 +3332,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C58" t="s">
         <v>133</v>
-      </c>
-      <c r="C58" t="s">
-        <v>134</v>
       </c>
       <c r="D58" t="s">
         <v>12</v>
@@ -3369,16 +3345,16 @@
       </c>
       <c r="F58" s="13"/>
       <c r="G58" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3386,28 +3362,28 @@
         <v>58</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C59" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D59" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3415,19 +3391,19 @@
         <v>59</v>
       </c>
       <c r="B60" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C60" t="s">
+        <v>319</v>
+      </c>
+      <c r="D60" t="s">
+        <v>22</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F60" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="C60" t="s">
-        <v>320</v>
-      </c>
-      <c r="D60" t="s">
-        <v>22</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>137</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>20</v>
@@ -3447,10 +3423,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C61" t="s">
         <v>138</v>
-      </c>
-      <c r="C61" t="s">
-        <v>139</v>
       </c>
       <c r="D61" t="s">
         <v>12</v>
@@ -3459,16 +3435,16 @@
         <v>13</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -3476,10 +3452,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C62" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D62" t="s">
         <v>22</v>
@@ -3488,16 +3464,16 @@
         <v>13</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -3505,10 +3481,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C63" t="s">
         <v>141</v>
-      </c>
-      <c r="C63" t="s">
-        <v>142</v>
       </c>
       <c r="D63" t="s">
         <v>12</v>
@@ -3517,16 +3493,16 @@
         <v>13</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -3534,10 +3510,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C64" t="s">
         <v>143</v>
-      </c>
-      <c r="C64" t="s">
-        <v>144</v>
       </c>
       <c r="D64" t="s">
         <v>12</v>
@@ -3546,16 +3522,16 @@
         <v>13</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
@@ -3563,19 +3539,19 @@
         <v>64</v>
       </c>
       <c r="B65" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C65" t="s">
+        <v>284</v>
+      </c>
+      <c r="D65" t="s">
+        <v>22</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="7" t="s">
         <v>145</v>
-      </c>
-      <c r="C65" t="s">
-        <v>285</v>
-      </c>
-      <c r="D65" t="s">
-        <v>22</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F65" s="7" t="s">
-        <v>146</v>
       </c>
       <c r="G65" s="7" t="s">
         <v>20</v>
@@ -3595,10 +3571,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C66" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D66" t="s">
         <v>22</v>
@@ -3607,7 +3583,7 @@
         <v>13</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G66" s="7" t="s">
         <v>20</v>
@@ -3628,10 +3604,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C67" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D67" t="s">
         <v>22</v>
@@ -3640,7 +3616,7 @@
         <v>13</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G67" s="7" t="s">
         <v>20</v>
@@ -3661,10 +3637,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C68" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D68" t="s">
         <v>22</v>
@@ -3673,7 +3649,7 @@
         <v>13</v>
       </c>
       <c r="F68" s="15" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G68" s="7" t="s">
         <v>20</v>
@@ -3686,7 +3662,7 @@
         <v>15</v>
       </c>
       <c r="K68" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="69" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3694,10 +3670,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C69" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D69" t="s">
         <v>22</v>
@@ -3707,17 +3683,17 @@
       </c>
       <c r="F69" s="9"/>
       <c r="G69" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I69"/>
       <c r="J69" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -3725,10 +3701,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C70" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D70" t="s">
         <v>22</v>
@@ -3738,17 +3714,17 @@
       </c>
       <c r="F70" s="7"/>
       <c r="G70" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I70" s="7"/>
       <c r="J70" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K70" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
@@ -3756,10 +3732,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C71" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D71" t="s">
         <v>22</v>
@@ -3769,17 +3745,17 @@
       </c>
       <c r="F71" s="7"/>
       <c r="G71" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H71" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I71" s="7"/>
       <c r="J71" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K71" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
@@ -3787,10 +3763,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C72" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D72" t="s">
         <v>22</v>
@@ -3800,17 +3776,17 @@
       </c>
       <c r="F72" s="7"/>
       <c r="G72" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H72" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I72" s="7"/>
       <c r="J72" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K72" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
@@ -3818,10 +3794,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C73" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D73" t="s">
         <v>22</v>
@@ -3831,17 +3807,17 @@
       </c>
       <c r="F73" s="7"/>
       <c r="G73" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H73" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I73" s="7"/>
       <c r="J73" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K73" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
@@ -3849,10 +3825,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C74" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D74" t="s">
         <v>22</v>
@@ -3862,17 +3838,17 @@
       </c>
       <c r="F74" s="7"/>
       <c r="G74" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H74" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I74" s="7"/>
       <c r="J74" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K74" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -3880,10 +3856,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C75" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D75" t="s">
         <v>22</v>
@@ -3892,7 +3868,7 @@
         <v>13</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G75" s="7" t="s">
         <v>20</v>
@@ -3913,10 +3889,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C76" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D76" t="s">
         <v>22</v>
@@ -3926,17 +3902,17 @@
       </c>
       <c r="F76" s="7"/>
       <c r="G76" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H76" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I76" s="7"/>
       <c r="J76" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K76" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="77" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3944,19 +3920,19 @@
         <v>76</v>
       </c>
       <c r="B77" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C77" t="s">
+        <v>296</v>
+      </c>
+      <c r="D77" t="s">
+        <v>22</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F77" s="13" t="s">
         <v>158</v>
-      </c>
-      <c r="C77" t="s">
-        <v>297</v>
-      </c>
-      <c r="D77" t="s">
-        <v>22</v>
-      </c>
-      <c r="E77" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F77" s="13" t="s">
-        <v>159</v>
       </c>
       <c r="G77" s="7" t="s">
         <v>20</v>
@@ -3965,13 +3941,13 @@
         <v>20</v>
       </c>
       <c r="I77" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J77" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K77" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="78" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3979,10 +3955,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C78" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D78" t="s">
         <v>22</v>
@@ -3991,7 +3967,7 @@
         <v>13</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G78" s="7" t="s">
         <v>20</v>
@@ -4012,19 +3988,19 @@
         <v>78</v>
       </c>
       <c r="B79" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C79" t="s">
         <v>162</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
+        <v>22</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F79" s="7" t="s">
         <v>163</v>
-      </c>
-      <c r="D79" t="s">
-        <v>22</v>
-      </c>
-      <c r="E79" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>164</v>
       </c>
       <c r="G79" s="7" t="s">
         <v>20</v>
@@ -4045,25 +4021,25 @@
         <v>79</v>
       </c>
       <c r="B80" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C80" t="s">
         <v>165</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D80" t="s">
+        <v>22</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F80" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="D80" t="s">
-        <v>22</v>
-      </c>
-      <c r="E80" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F80" s="7" t="s">
+      <c r="G80" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H80" s="7" t="s">
         <v>167</v>
-      </c>
-      <c r="G80" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H80" s="7" t="s">
-        <v>168</v>
       </c>
       <c r="I80" s="7"/>
       <c r="J80" s="7" t="s">
@@ -4078,25 +4054,25 @@
         <v>80</v>
       </c>
       <c r="B81" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C81" t="s">
         <v>169</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
+        <v>22</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F81" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D81" t="s">
-        <v>22</v>
-      </c>
-      <c r="E81" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F81" s="7" t="s">
+      <c r="G81" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H81" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="G81" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H81" s="7" t="s">
-        <v>172</v>
       </c>
       <c r="I81" s="7"/>
       <c r="J81" s="7" t="s">
@@ -4111,25 +4087,25 @@
         <v>81</v>
       </c>
       <c r="B82" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C82" t="s">
         <v>173</v>
       </c>
-      <c r="C82" t="s">
+      <c r="D82" t="s">
+        <v>22</v>
+      </c>
+      <c r="E82" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F82" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="D82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E82" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F82" s="7" t="s">
+      <c r="G82" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H82" s="7" t="s">
         <v>175</v>
-      </c>
-      <c r="G82" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H82" s="7" t="s">
-        <v>176</v>
       </c>
       <c r="I82" s="7"/>
       <c r="J82" s="7" t="s">
@@ -4144,25 +4120,25 @@
         <v>82</v>
       </c>
       <c r="B83" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C83" t="s">
         <v>177</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
+        <v>22</v>
+      </c>
+      <c r="E83" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F83" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="D83" t="s">
-        <v>22</v>
-      </c>
-      <c r="E83" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F83" s="7" t="s">
+      <c r="G83" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H83" s="7" t="s">
         <v>179</v>
-      </c>
-      <c r="G83" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H83" s="7" t="s">
-        <v>180</v>
       </c>
       <c r="I83" s="7"/>
       <c r="J83" s="7" t="s">
@@ -4177,25 +4153,25 @@
         <v>83</v>
       </c>
       <c r="B84" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C84" t="s">
         <v>181</v>
       </c>
-      <c r="C84" t="s">
+      <c r="D84" t="s">
+        <v>22</v>
+      </c>
+      <c r="E84" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F84" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="D84" t="s">
-        <v>22</v>
-      </c>
-      <c r="E84" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F84" s="7" t="s">
+      <c r="G84" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H84" s="7" t="s">
         <v>183</v>
-      </c>
-      <c r="G84" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H84" s="7" t="s">
-        <v>184</v>
       </c>
       <c r="I84" s="7"/>
       <c r="J84" s="7" t="s">
@@ -4210,25 +4186,25 @@
         <v>84</v>
       </c>
       <c r="B85" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C85" t="s">
         <v>185</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D85" t="s">
+        <v>22</v>
+      </c>
+      <c r="E85" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F85" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="D85" t="s">
-        <v>22</v>
-      </c>
-      <c r="E85" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F85" s="7" t="s">
+      <c r="G85" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H85" s="7" t="s">
         <v>187</v>
-      </c>
-      <c r="G85" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H85" s="7" t="s">
-        <v>188</v>
       </c>
       <c r="I85" s="7"/>
       <c r="J85" s="7" t="s">
@@ -4243,25 +4219,25 @@
         <v>85</v>
       </c>
       <c r="B86" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C86" t="s">
         <v>189</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
+        <v>22</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F86" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="D86" t="s">
-        <v>22</v>
-      </c>
-      <c r="E86" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F86" s="7" t="s">
+      <c r="G86" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H86" s="7" t="s">
         <v>191</v>
-      </c>
-      <c r="G86" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H86" s="7" t="s">
-        <v>192</v>
       </c>
       <c r="I86" s="7"/>
       <c r="J86" s="7" t="s">
@@ -4276,25 +4252,25 @@
         <v>86</v>
       </c>
       <c r="B87" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C87" t="s">
         <v>193</v>
       </c>
-      <c r="C87" t="s">
+      <c r="D87" t="s">
+        <v>22</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F87" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="D87" t="s">
-        <v>22</v>
-      </c>
-      <c r="E87" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F87" s="7" t="s">
+      <c r="G87" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H87" s="7" t="s">
         <v>195</v>
-      </c>
-      <c r="G87" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H87" s="7" t="s">
-        <v>196</v>
       </c>
       <c r="I87" s="7"/>
       <c r="J87" s="7" t="s">
@@ -4309,10 +4285,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C88" t="s">
         <v>197</v>
-      </c>
-      <c r="C88" t="s">
-        <v>198</v>
       </c>
       <c r="D88" t="s">
         <v>22</v>
@@ -4322,17 +4298,17 @@
       </c>
       <c r="F88" s="7"/>
       <c r="G88" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H88" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I88" s="7"/>
       <c r="J88" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K88" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
@@ -4340,10 +4316,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C89" t="s">
         <v>199</v>
-      </c>
-      <c r="C89" t="s">
-        <v>200</v>
       </c>
       <c r="D89" t="s">
         <v>22</v>
@@ -4353,17 +4329,17 @@
       </c>
       <c r="F89" s="7"/>
       <c r="G89" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H89" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I89" s="7"/>
       <c r="J89" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K89" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
@@ -4371,10 +4347,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C90" t="s">
         <v>201</v>
-      </c>
-      <c r="C90" t="s">
-        <v>202</v>
       </c>
       <c r="D90" t="s">
         <v>22</v>
@@ -4384,17 +4360,17 @@
       </c>
       <c r="F90" s="7"/>
       <c r="G90" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I90" s="7"/>
       <c r="J90" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K90" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
@@ -4402,25 +4378,25 @@
         <v>90</v>
       </c>
       <c r="B91" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C91" t="s">
         <v>203</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
+        <v>22</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F91" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="D91" t="s">
-        <v>22</v>
-      </c>
-      <c r="E91" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F91" s="7" t="s">
+      <c r="G91" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H91" s="7" t="s">
         <v>205</v>
-      </c>
-      <c r="G91" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H91" s="7" t="s">
-        <v>206</v>
       </c>
       <c r="I91" s="7"/>
       <c r="J91" s="7" t="s">
@@ -4435,25 +4411,25 @@
         <v>91</v>
       </c>
       <c r="B92" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C92" t="s">
         <v>207</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D92" t="s">
+        <v>22</v>
+      </c>
+      <c r="E92" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F92" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="D92" t="s">
-        <v>22</v>
-      </c>
-      <c r="E92" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F92" s="7" t="s">
+      <c r="G92" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H92" s="7" t="s">
         <v>209</v>
-      </c>
-      <c r="G92" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H92" s="7" t="s">
-        <v>210</v>
       </c>
       <c r="I92" s="7"/>
       <c r="J92" s="7" t="s">
@@ -4468,11 +4444,11 @@
         <v>92</v>
       </c>
       <c r="B93" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C93" t="s">
         <v>211</v>
       </c>
-      <c r="C93" t="s">
-        <v>212</v>
-      </c>
       <c r="D93" t="s">
         <v>22</v>
       </c>
@@ -4480,7 +4456,7 @@
         <v>13</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>20</v>
@@ -4489,7 +4465,7 @@
         <v>20</v>
       </c>
       <c r="I93" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J93" s="7" t="s">
         <v>15</v>
@@ -4503,10 +4479,10 @@
         <v>93</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C94" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D94" t="s">
         <v>22</v>
@@ -4515,7 +4491,7 @@
         <v>13</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>20</v>
@@ -4524,7 +4500,7 @@
         <v>20</v>
       </c>
       <c r="I94" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J94" s="7" t="s">
         <v>15</v>
@@ -4538,19 +4514,19 @@
         <v>94</v>
       </c>
       <c r="B95" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C95" t="s">
+        <v>321</v>
+      </c>
+      <c r="D95" t="s">
+        <v>22</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F95" s="7" t="s">
         <v>215</v>
-      </c>
-      <c r="C95" t="s">
-        <v>322</v>
-      </c>
-      <c r="D95" t="s">
-        <v>22</v>
-      </c>
-      <c r="E95" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F95" s="7" t="s">
-        <v>216</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>20</v>
@@ -4571,25 +4547,25 @@
         <v>95</v>
       </c>
       <c r="B96" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C96" t="s">
+        <v>322</v>
+      </c>
+      <c r="D96" t="s">
+        <v>22</v>
+      </c>
+      <c r="E96" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F96" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="C96" t="s">
-        <v>323</v>
-      </c>
-      <c r="D96" t="s">
-        <v>22</v>
-      </c>
-      <c r="E96" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F96" s="7" t="s">
+      <c r="G96" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H96" s="7" t="s">
         <v>218</v>
-      </c>
-      <c r="G96" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H96" s="7" t="s">
-        <v>219</v>
       </c>
       <c r="I96" s="7"/>
       <c r="J96" s="7" t="s">
@@ -4604,32 +4580,32 @@
         <v>96</v>
       </c>
       <c r="B97" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C97" t="s">
         <v>220</v>
       </c>
-      <c r="C97" t="s">
+      <c r="D97" t="s">
+        <v>22</v>
+      </c>
+      <c r="E97" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F97" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="G97" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H97" s="15" t="s">
         <v>221</v>
-      </c>
-      <c r="D97" t="s">
-        <v>22</v>
-      </c>
-      <c r="E97" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F97" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="G97" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H97" s="15" t="s">
-        <v>222</v>
       </c>
       <c r="I97" s="7"/>
       <c r="J97" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K97" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="98" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -4637,10 +4613,10 @@
         <v>97</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C98" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D98" t="s">
         <v>22</v>
@@ -4649,20 +4625,20 @@
         <v>13</v>
       </c>
       <c r="F98" s="15" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G98" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H98" s="15" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I98" s="7"/>
       <c r="J98" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K98" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
@@ -4670,32 +4646,32 @@
         <v>98</v>
       </c>
       <c r="B99" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="C99" t="s">
+        <v>300</v>
+      </c>
+      <c r="D99" t="s">
+        <v>22</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F99" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="C99" t="s">
-        <v>301</v>
-      </c>
-      <c r="D99" t="s">
-        <v>22</v>
-      </c>
-      <c r="E99" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F99" s="7" t="s">
+      <c r="G99" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H99" s="7" t="s">
         <v>225</v>
-      </c>
-      <c r="G99" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H99" s="7" t="s">
-        <v>226</v>
       </c>
       <c r="I99" s="7"/>
       <c r="J99" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K99" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
@@ -4703,32 +4679,32 @@
         <v>99</v>
       </c>
       <c r="B100" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C100" t="s">
+        <v>301</v>
+      </c>
+      <c r="D100" t="s">
+        <v>22</v>
+      </c>
+      <c r="E100" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F100" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="C100" t="s">
-        <v>302</v>
-      </c>
-      <c r="D100" t="s">
-        <v>22</v>
-      </c>
-      <c r="E100" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F100" s="7" t="s">
+      <c r="G100" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H100" s="7" t="s">
         <v>228</v>
-      </c>
-      <c r="G100" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H100" s="7" t="s">
-        <v>229</v>
       </c>
       <c r="I100" s="7"/>
       <c r="J100" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K100" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
@@ -4736,10 +4712,10 @@
         <v>100</v>
       </c>
       <c r="B101" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="C101" t="s">
         <v>230</v>
-      </c>
-      <c r="C101" t="s">
-        <v>231</v>
       </c>
       <c r="D101" t="s">
         <v>22</v>
@@ -4749,17 +4725,17 @@
       </c>
       <c r="F101" s="7"/>
       <c r="G101" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I101" s="7"/>
       <c r="J101" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K101" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
@@ -4767,32 +4743,32 @@
         <v>101</v>
       </c>
       <c r="B102" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C102" t="s">
         <v>232</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D102" t="s">
+        <v>22</v>
+      </c>
+      <c r="E102" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F102" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="D102" t="s">
-        <v>22</v>
-      </c>
-      <c r="E102" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F102" s="7" t="s">
+      <c r="G102" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H102" s="7" t="s">
         <v>234</v>
-      </c>
-      <c r="G102" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H102" s="7" t="s">
-        <v>235</v>
       </c>
       <c r="I102" s="7"/>
       <c r="J102" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K102" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
@@ -4800,10 +4776,10 @@
         <v>102</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C103" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D103" t="s">
         <v>22</v>
@@ -4813,17 +4789,17 @@
       </c>
       <c r="F103" s="7"/>
       <c r="G103" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H103" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I103" s="7"/>
       <c r="J103" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K103" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="104" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -4831,10 +4807,10 @@
         <v>103</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C104" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D104" t="s">
         <v>22</v>
@@ -4843,20 +4819,20 @@
         <v>13</v>
       </c>
       <c r="F104" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="G104" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H104" s="15" t="s">
         <v>258</v>
-      </c>
-      <c r="G104" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H104" s="15" t="s">
-        <v>259</v>
       </c>
       <c r="I104" s="7"/>
       <c r="J104" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K104" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
@@ -4864,11 +4840,11 @@
         <v>104</v>
       </c>
       <c r="B105" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="C105" t="s">
         <v>238</v>
       </c>
-      <c r="C105" t="s">
-        <v>239</v>
-      </c>
       <c r="D105" t="s">
         <v>22</v>
       </c>
@@ -4876,20 +4852,20 @@
         <v>13</v>
       </c>
       <c r="F105" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="G105" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H105" s="7" t="s">
         <v>260</v>
-      </c>
-      <c r="G105" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H105" s="7" t="s">
-        <v>261</v>
       </c>
       <c r="I105" s="7"/>
       <c r="J105" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K105" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
@@ -4897,32 +4873,32 @@
         <v>105</v>
       </c>
       <c r="B106" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="C106" t="s">
         <v>240</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D106" t="s">
+        <v>22</v>
+      </c>
+      <c r="E106" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F106" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="D106" t="s">
-        <v>22</v>
-      </c>
-      <c r="E106" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F106" s="7" t="s">
+      <c r="G106" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H106" s="7" t="s">
         <v>242</v>
-      </c>
-      <c r="G106" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H106" s="7" t="s">
-        <v>243</v>
       </c>
       <c r="I106" s="7"/>
       <c r="J106" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K106" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
@@ -4930,10 +4906,10 @@
         <v>106</v>
       </c>
       <c r="B107" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C107" t="s">
         <v>244</v>
-      </c>
-      <c r="C107" t="s">
-        <v>245</v>
       </c>
       <c r="D107" t="s">
         <v>22</v>
@@ -4943,17 +4919,17 @@
       </c>
       <c r="F107" s="7"/>
       <c r="G107" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H107" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I107" s="7"/>
       <c r="J107" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K107" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
@@ -4961,19 +4937,19 @@
         <v>107</v>
       </c>
       <c r="B108" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C108" t="s">
         <v>246</v>
       </c>
-      <c r="C108" t="s">
+      <c r="D108" t="s">
+        <v>22</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F108" s="7" t="s">
         <v>247</v>
-      </c>
-      <c r="D108" t="s">
-        <v>22</v>
-      </c>
-      <c r="E108" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F108" s="7" t="s">
-        <v>248</v>
       </c>
       <c r="G108" s="7" t="s">
         <v>20</v>
@@ -4994,10 +4970,10 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
+        <v>248</v>
+      </c>
+      <c r="C109" t="s">
         <v>249</v>
-      </c>
-      <c r="C109" t="s">
-        <v>250</v>
       </c>
       <c r="D109" t="s">
         <v>12</v>
@@ -5006,16 +4982,16 @@
         <v>13</v>
       </c>
       <c r="F109" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="G109" s="3" t="s">
         <v>251</v>
-      </c>
-      <c r="G109" s="3" t="s">
-        <v>252</v>
       </c>
       <c r="H109">
         <v>1</v>
       </c>
       <c r="I109" s="24" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J109" s="12" t="s">
         <v>15</v>
@@ -5097,6 +5073,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -5337,7 +5325,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -5346,19 +5334,18 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF2265-5030-4B54-A34F-4798AFD4DA4C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2AE2FD3-517E-4530-8BC5-1FF35C67F615}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5377,21 +5364,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{398CA3EE-638E-435F-8CA6-D67A7B863103}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FADF2265-5030-4B54-A34F-4798AFD4DA4C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>